<commit_message>
Fixed errors in the data
</commit_message>
<xml_diff>
--- a/data/JCOMSS/results_model1a.xlsx
+++ b/data/JCOMSS/results_model1a.xlsx
@@ -1573,25 +1573,25 @@
         <v>0.5</v>
       </c>
       <c r="AI3" t="n" s="83">
-        <v>0.9988639504366098</v>
+        <v>0.9986038038365268</v>
       </c>
       <c r="AJ3" t="n" s="83">
-        <v>0.9999217332665077</v>
+        <v>0.9996255037472908</v>
       </c>
       <c r="AK3" t="n" s="83">
-        <v>0.9999825180410691</v>
+        <v>1.0</v>
       </c>
       <c r="AL3" t="n" s="83">
-        <v>0.9970698439175792</v>
+        <v>0.9924006565224265</v>
       </c>
       <c r="AM3" t="n" s="83">
-        <v>0.9992866611469318</v>
+        <v>1.0</v>
       </c>
       <c r="AN3" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO3" t="n" s="83">
-        <v>0.8989148535057891</v>
+        <v>1.0</v>
       </c>
       <c r="AP3" t="n" s="83">
         <v>1.0</v>
@@ -1695,25 +1695,25 @@
         <v>0.5</v>
       </c>
       <c r="AI4" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ4" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999912182350975</v>
       </c>
       <c r="AK4" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>1.0</v>
       </c>
       <c r="AL4" t="n" s="83">
-        <v>0.9997133626502709</v>
+        <v>0.9991534821357767</v>
       </c>
       <c r="AM4" t="n" s="83">
-        <v>0.9999999996269755</v>
+        <v>1.0</v>
       </c>
       <c r="AN4" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO4" t="n" s="83">
-        <v>0.9997361565408506</v>
+        <v>1.0</v>
       </c>
       <c r="AP4" t="n" s="83">
         <v>1.0</v>
@@ -1817,25 +1817,25 @@
         <v>0.5</v>
       </c>
       <c r="AI5" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ5" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK5" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL5" t="n" s="83">
-        <v>0.9999634386555672</v>
+        <v>0.9998455303631983</v>
       </c>
       <c r="AM5" t="n" s="83">
-        <v>0.9999999999999951</v>
+        <v>1.0</v>
       </c>
       <c r="AN5" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO5" t="n" s="83">
-        <v>0.9999907736430119</v>
+        <v>1.0</v>
       </c>
       <c r="AP5" t="n" s="83">
         <v>1.0</v>
@@ -1939,25 +1939,25 @@
         <v>0.5</v>
       </c>
       <c r="AI6" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ6" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK6" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL6" t="n" s="83">
-        <v>0.9999744279750036</v>
+        <v>0.9998919557943996</v>
       </c>
       <c r="AM6" t="n" s="83">
-        <v>0.9999999999999984</v>
+        <v>1.0</v>
       </c>
       <c r="AN6" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO6" t="n" s="83">
-        <v>0.9999987328523009</v>
+        <v>1.0</v>
       </c>
       <c r="AP6" t="n" s="83">
         <v>1.0</v>
@@ -2061,25 +2061,25 @@
         <v>0.5</v>
       </c>
       <c r="AI7" t="n" s="83">
-        <v>0.9991274378874396</v>
+        <v>0.9989275631034111</v>
       </c>
       <c r="AJ7" t="n" s="83">
-        <v>0.9999984732404491</v>
+        <v>0.9999926925293007</v>
       </c>
       <c r="AK7" t="n" s="83">
-        <v>0.9999999999024841</v>
+        <v>1.0</v>
       </c>
       <c r="AL7" t="n" s="83">
-        <v>0.9999264291745467</v>
+        <v>0.9997252734072887</v>
       </c>
       <c r="AM7" t="n" s="83">
-        <v>0.9999999999927577</v>
+        <v>1.0</v>
       </c>
       <c r="AN7" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO7" t="n" s="83">
-        <v>0.9999346317783462</v>
+        <v>1.0</v>
       </c>
       <c r="AP7" t="n" s="83">
         <v>1.0</v>
@@ -2183,28 +2183,28 @@
         <v>0.5</v>
       </c>
       <c r="AI8" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ8" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999988177650597</v>
       </c>
       <c r="AK8" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>0.9999999999922596</v>
       </c>
       <c r="AL8" t="n" s="83">
-        <v>0.9993744113189219</v>
+        <v>0.9995365738711016</v>
       </c>
       <c r="AM8" t="n" s="83">
-        <v>0.9999999951354414</v>
+        <v>0.9999999981342332</v>
       </c>
       <c r="AN8" t="n" s="83">
-        <v>0.9999999995857503</v>
+        <v>1.0</v>
       </c>
       <c r="AO8" t="n" s="83">
-        <v>0.9804205571019377</v>
+        <v>0.9772906224640616</v>
       </c>
       <c r="AP8" t="n" s="83">
-        <v>0.9918645376684081</v>
+        <v>0.9976725598593037</v>
       </c>
       <c r="AQ8" t="n" s="83">
         <v>0.44683149221674895</v>
@@ -2305,25 +2305,25 @@
         <v>0.5</v>
       </c>
       <c r="AI9" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ9" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK9" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL9" t="n" s="83">
-        <v>0.9999845703437606</v>
+        <v>0.9999348061217294</v>
       </c>
       <c r="AM9" t="n" s="83">
-        <v>0.9999999999999997</v>
+        <v>1.0</v>
       </c>
       <c r="AN9" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO9" t="n" s="83">
-        <v>0.9999998841222452</v>
+        <v>1.0</v>
       </c>
       <c r="AP9" t="n" s="83">
         <v>1.0</v>
@@ -2427,25 +2427,25 @@
         <v>0.5</v>
       </c>
       <c r="AI10" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9988625441701168</v>
       </c>
       <c r="AJ10" t="n" s="83">
-        <v>0.9999986664649917</v>
+        <v>0.9999936173478504</v>
       </c>
       <c r="AK10" t="n" s="83">
-        <v>0.999999999959948</v>
+        <v>1.0</v>
       </c>
       <c r="AL10" t="n" s="83">
-        <v>0.9998904968932578</v>
+        <v>0.9996355503714819</v>
       </c>
       <c r="AM10" t="n" s="83">
-        <v>0.9999999999963215</v>
+        <v>1.0</v>
       </c>
       <c r="AN10" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO10" t="n" s="83">
-        <v>0.9999799237824233</v>
+        <v>1.0</v>
       </c>
       <c r="AP10" t="n" s="83">
         <v>1.0</v>
@@ -2549,25 +2549,25 @@
         <v>0.5</v>
       </c>
       <c r="AI11" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ11" t="n" s="83">
-        <v>0.9999962581098016</v>
+        <v>0.9999820904846234</v>
       </c>
       <c r="AK11" t="n" s="83">
-        <v>0.999999922498761</v>
+        <v>1.0</v>
       </c>
       <c r="AL11" t="n" s="83">
-        <v>0.9999733663354602</v>
+        <v>0.9998874706529893</v>
       </c>
       <c r="AM11" t="n" s="83">
-        <v>0.9999999994625067</v>
+        <v>1.0</v>
       </c>
       <c r="AN11" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO11" t="n" s="83">
-        <v>0.9999325280534376</v>
+        <v>1.0</v>
       </c>
       <c r="AP11" t="n" s="83">
         <v>1.0</v>
@@ -2671,25 +2671,25 @@
         <v>0.5</v>
       </c>
       <c r="AI12" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ12" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK12" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL12" t="n" s="83">
-        <v>0.9999845703437606</v>
+        <v>0.9999348061217294</v>
       </c>
       <c r="AM12" t="n" s="83">
-        <v>0.9999999999999997</v>
+        <v>1.0</v>
       </c>
       <c r="AN12" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO12" t="n" s="83">
-        <v>0.9999998841222452</v>
+        <v>1.0</v>
       </c>
       <c r="AP12" t="n" s="83">
         <v>1.0</v>
@@ -2793,25 +2793,25 @@
         <v>0.5</v>
       </c>
       <c r="AI13" t="n" s="83">
-        <v>0.9991493793904361</v>
+        <v>0.9989545254113691</v>
       </c>
       <c r="AJ13" t="n" s="83">
-        <v>0.9969794481525968</v>
+        <v>0.985706238159561</v>
       </c>
       <c r="AK13" t="n" s="83">
-        <v>0.5669187101124126</v>
+        <v>1.0</v>
       </c>
       <c r="AL13" t="n" s="83">
-        <v>0.9998959364107073</v>
+        <v>0.9996098141562775</v>
       </c>
       <c r="AM13" t="n" s="83">
-        <v>0.9999310123561127</v>
+        <v>1.0</v>
       </c>
       <c r="AN13" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO13" t="n" s="83">
-        <v>0.9999798278939418</v>
+        <v>1.0</v>
       </c>
       <c r="AP13" t="n" s="83">
         <v>1.0</v>
@@ -2915,28 +2915,28 @@
         <v>0.5</v>
       </c>
       <c r="AI14" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9993455450789266</v>
       </c>
       <c r="AJ14" t="n" s="83">
-        <v>0.9999710701574831</v>
+        <v>0.9999813590445108</v>
       </c>
       <c r="AK14" t="n" s="83">
-        <v>0.9633828822826286</v>
+        <v>0.9863097136064665</v>
       </c>
       <c r="AL14" t="n" s="83">
-        <v>0.99996299736163</v>
+        <v>0.9999761572668473</v>
       </c>
       <c r="AM14" t="n" s="83">
-        <v>0.9999228270695063</v>
+        <v>0.999993388016971</v>
       </c>
       <c r="AN14" t="n" s="83">
-        <v>0.6652442937456171</v>
+        <v>0.9999999999999981</v>
       </c>
       <c r="AO14" t="n" s="83">
-        <v>0.9253116744831718</v>
+        <v>0.9604108736216355</v>
       </c>
       <c r="AP14" t="n" s="83">
-        <v>0.18649633698327567</v>
+        <v>0.9999998857851365</v>
       </c>
       <c r="AQ14" t="n" s="83">
         <v>4.527253923894539E-18</v>
@@ -3037,25 +3037,25 @@
         <v>0.5</v>
       </c>
       <c r="AI15" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ15" t="n" s="83">
-        <v>0.9999919193686365</v>
+        <v>0.9999613249436422</v>
       </c>
       <c r="AK15" t="n" s="83">
-        <v>0.9998555831295834</v>
+        <v>1.0</v>
       </c>
       <c r="AL15" t="n" s="83">
-        <v>0.9997133626502709</v>
+        <v>0.9991534821357767</v>
       </c>
       <c r="AM15" t="n" s="83">
-        <v>0.9991712963818669</v>
+        <v>1.0</v>
       </c>
       <c r="AN15" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO15" t="n" s="83">
-        <v>0.9552683743192182</v>
+        <v>1.0</v>
       </c>
       <c r="AP15" t="n" s="83">
         <v>1.0</v>
@@ -3159,28 +3159,28 @@
         <v>0.5</v>
       </c>
       <c r="AI16" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9993455450789266</v>
       </c>
       <c r="AJ16" t="n" s="83">
-        <v>0.9999933737059371</v>
+        <v>0.9999957303786636</v>
       </c>
       <c r="AK16" t="n" s="83">
-        <v>0.9999999570501501</v>
+        <v>0.9999999939194247</v>
       </c>
       <c r="AL16" t="n" s="83">
-        <v>0.9999928437010657</v>
+        <v>0.9999953888716544</v>
       </c>
       <c r="AM16" t="n" s="83">
-        <v>0.9999999999998656</v>
+        <v>0.9999999999999742</v>
       </c>
       <c r="AN16" t="n" s="83">
-        <v>0.999999998939674</v>
+        <v>1.0</v>
       </c>
       <c r="AO16" t="n" s="83">
-        <v>0.999999862195202</v>
+        <v>0.9999999726490066</v>
       </c>
       <c r="AP16" t="n" s="83">
-        <v>0.9999999933647311</v>
+        <v>1.0</v>
       </c>
       <c r="AQ16" t="n" s="83">
         <v>0.9996144106340238</v>
@@ -3281,25 +3281,25 @@
         <v>0.5</v>
       </c>
       <c r="AI17" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9988625441701168</v>
       </c>
       <c r="AJ17" t="n" s="83">
-        <v>0.9999986664649917</v>
+        <v>0.9999936173478504</v>
       </c>
       <c r="AK17" t="n" s="83">
-        <v>0.999999999959948</v>
+        <v>1.0</v>
       </c>
       <c r="AL17" t="n" s="83">
-        <v>0.9998860506821844</v>
+        <v>0.9996207563616588</v>
       </c>
       <c r="AM17" t="n" s="83">
-        <v>0.9999999999959899</v>
+        <v>1.0</v>
       </c>
       <c r="AN17" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO17" t="n" s="83">
-        <v>0.9999774288148149</v>
+        <v>1.0</v>
       </c>
       <c r="AP17" t="n" s="83">
         <v>1.0</v>
@@ -3403,16 +3403,16 @@
         <v>0.5</v>
       </c>
       <c r="AI18" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ18" t="n" s="83">
-        <v>0.9999995379719052</v>
+        <v>0.9999977886037303</v>
       </c>
       <c r="AK18" t="n" s="83">
-        <v>0.9999999999999568</v>
+        <v>1.0</v>
       </c>
       <c r="AL18" t="n" s="83">
-        <v>0.999992230858993</v>
+        <v>0.9999628157371441</v>
       </c>
       <c r="AM18" t="n" s="83">
         <v>1.0</v>
@@ -3421,7 +3421,7 @@
         <v>1.0</v>
       </c>
       <c r="AO18" t="n" s="83">
-        <v>0.9999999218192753</v>
+        <v>1.0</v>
       </c>
       <c r="AP18" t="n" s="83">
         <v>1.0</v>
@@ -3525,25 +3525,25 @@
         <v>0.5</v>
       </c>
       <c r="AI19" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ19" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK19" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL19" t="n" s="83">
-        <v>0.9999744279750036</v>
+        <v>0.9998919557943996</v>
       </c>
       <c r="AM19" t="n" s="83">
-        <v>0.9999999999999984</v>
+        <v>1.0</v>
       </c>
       <c r="AN19" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO19" t="n" s="83">
-        <v>0.9999987328523009</v>
+        <v>1.0</v>
       </c>
       <c r="AP19" t="n" s="83">
         <v>1.0</v>
@@ -3647,25 +3647,25 @@
         <v>0.5</v>
       </c>
       <c r="AI20" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ20" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK20" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL20" t="n" s="83">
-        <v>0.9999634386555672</v>
+        <v>0.9998455303631983</v>
       </c>
       <c r="AM20" t="n" s="83">
-        <v>0.9999999999999951</v>
+        <v>1.0</v>
       </c>
       <c r="AN20" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO20" t="n" s="83">
-        <v>0.9999907736430119</v>
+        <v>1.0</v>
       </c>
       <c r="AP20" t="n" s="83">
         <v>1.0</v>
@@ -3769,16 +3769,16 @@
         <v>0.5</v>
       </c>
       <c r="AI21" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ21" t="n" s="83">
-        <v>0.9999995379719052</v>
+        <v>0.9999977886037303</v>
       </c>
       <c r="AK21" t="n" s="83">
-        <v>0.9999999999999568</v>
+        <v>1.0</v>
       </c>
       <c r="AL21" t="n" s="83">
-        <v>0.9999950388597546</v>
+        <v>0.9999762549934307</v>
       </c>
       <c r="AM21" t="n" s="83">
         <v>1.0</v>
@@ -3787,7 +3787,7 @@
         <v>1.0</v>
       </c>
       <c r="AO21" t="n" s="83">
-        <v>0.9999999914859279</v>
+        <v>1.0</v>
       </c>
       <c r="AP21" t="n" s="83">
         <v>1.0</v>
@@ -3891,25 +3891,25 @@
         <v>0.5</v>
       </c>
       <c r="AI22" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ22" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK22" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL22" t="n" s="83">
-        <v>0.9999764198929206</v>
+        <v>0.9999003711945014</v>
       </c>
       <c r="AM22" t="n" s="83">
-        <v>0.9999999999999987</v>
+        <v>1.0</v>
       </c>
       <c r="AN22" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO22" t="n" s="83">
-        <v>0.99999899485984</v>
+        <v>1.0</v>
       </c>
       <c r="AP22" t="n" s="83">
         <v>1.0</v>
@@ -4013,16 +4013,16 @@
         <v>0.5</v>
       </c>
       <c r="AI23" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ23" t="n" s="83">
-        <v>0.9999995379719052</v>
+        <v>0.9999977886037303</v>
       </c>
       <c r="AK23" t="n" s="83">
-        <v>0.9999999999999568</v>
+        <v>1.0</v>
       </c>
       <c r="AL23" t="n" s="83">
-        <v>0.9999881215995371</v>
+        <v>0.9999431490955246</v>
       </c>
       <c r="AM23" t="n" s="83">
         <v>1.0</v>
@@ -4031,7 +4031,7 @@
         <v>1.0</v>
       </c>
       <c r="AO23" t="n" s="83">
-        <v>0.9999993218342604</v>
+        <v>1.0</v>
       </c>
       <c r="AP23" t="n" s="83">
         <v>1.0</v>
@@ -4135,25 +4135,25 @@
         <v>0.5</v>
       </c>
       <c r="AI24" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ24" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK24" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL24" t="n" s="83">
-        <v>0.9999764198929206</v>
+        <v>0.9999003711945014</v>
       </c>
       <c r="AM24" t="n" s="83">
-        <v>0.9999999999999987</v>
+        <v>1.0</v>
       </c>
       <c r="AN24" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO24" t="n" s="83">
-        <v>0.99999899485984</v>
+        <v>1.0</v>
       </c>
       <c r="AP24" t="n" s="83">
         <v>1.0</v>
@@ -4257,25 +4257,25 @@
         <v>0.5</v>
       </c>
       <c r="AI25" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ25" t="n" s="83">
-        <v>0.9999989604594058</v>
+        <v>0.9999950244775335</v>
       </c>
       <c r="AK25" t="n" s="83">
-        <v>0.9999999999889619</v>
+        <v>1.0</v>
       </c>
       <c r="AL25" t="n" s="83">
-        <v>0.9999634386555672</v>
+        <v>0.9998455303631983</v>
       </c>
       <c r="AM25" t="n" s="83">
-        <v>0.9999999999997394</v>
+        <v>1.0</v>
       </c>
       <c r="AN25" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO25" t="n" s="83">
-        <v>0.9999631525032587</v>
+        <v>1.0</v>
       </c>
       <c r="AP25" t="n" s="83">
         <v>1.0</v>
@@ -4379,25 +4379,25 @@
         <v>0.5</v>
       </c>
       <c r="AI26" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ26" t="n" s="83">
-        <v>0.9522935044601201</v>
+        <v>0.8065973460366054</v>
       </c>
       <c r="AK26" t="n" s="83">
-        <v>0.6892102215584675</v>
+        <v>1.0</v>
       </c>
       <c r="AL26" t="n" s="83">
-        <v>0.9827805113493441</v>
+        <v>0.950774743260213</v>
       </c>
       <c r="AM26" t="n" s="83">
-        <v>0.8981339055710925</v>
+        <v>1.0</v>
       </c>
       <c r="AN26" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO26" t="n" s="83">
-        <v>0.8606849747810309</v>
+        <v>1.0</v>
       </c>
       <c r="AP26" t="n" s="83">
         <v>1.0</v>
@@ -4501,28 +4501,28 @@
         <v>0.5</v>
       </c>
       <c r="AI27" t="n" s="83">
-        <v>0.9992488414630909</v>
+        <v>0.9992874728754778</v>
       </c>
       <c r="AJ27" t="n" s="83">
-        <v>0.9994328908555525</v>
+        <v>0.9996345130406405</v>
       </c>
       <c r="AK27" t="n" s="83">
-        <v>0.7436227406192696</v>
+        <v>0.8503996158235277</v>
       </c>
       <c r="AL27" t="n" s="83">
-        <v>0.9998547666653038</v>
+        <v>0.999903177817316</v>
       </c>
       <c r="AM27" t="n" s="83">
-        <v>0.999481752945598</v>
+        <v>0.9999470890337561</v>
       </c>
       <c r="AN27" t="n" s="83">
-        <v>0.002266401580341779</v>
+        <v>0.9999872869607344</v>
       </c>
       <c r="AO27" t="n" s="83">
-        <v>0.96216885034987</v>
+        <v>0.985514535038457</v>
       </c>
       <c r="AP27" t="n" s="83">
-        <v>0.15512066893808718</v>
+        <v>0.9999999999999749</v>
       </c>
       <c r="AQ27" t="n" s="83">
         <v>1.6844611136281664E-22</v>
@@ -4623,25 +4623,25 @@
         <v>0.5</v>
       </c>
       <c r="AI28" t="n" s="83">
-        <v>0.999039066803416</v>
+        <v>0.9988189730891767</v>
       </c>
       <c r="AJ28" t="n" s="83">
-        <v>0.9999978313666398</v>
+        <v>0.9999896203785227</v>
       </c>
       <c r="AK28" t="n" s="83">
-        <v>0.9999999990669062</v>
+        <v>1.0</v>
       </c>
       <c r="AL28" t="n" s="83">
-        <v>0.9998610326545109</v>
+        <v>0.9995405399550081</v>
       </c>
       <c r="AM28" t="n" s="83">
-        <v>0.9999999997959595</v>
+        <v>1.0</v>
       </c>
       <c r="AN28" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO28" t="n" s="83">
-        <v>0.9998896685160733</v>
+        <v>1.0</v>
       </c>
       <c r="AP28" t="n" s="83">
         <v>1.0</v>
@@ -4745,25 +4745,25 @@
         <v>0.5</v>
       </c>
       <c r="AI29" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9984827843506957</v>
       </c>
       <c r="AJ29" t="n" s="83">
-        <v>0.9999962083360194</v>
+        <v>0.9999818522596959</v>
       </c>
       <c r="AK29" t="n" s="83">
-        <v>0.9999999643406988</v>
+        <v>1.0</v>
       </c>
       <c r="AL29" t="n" s="83">
-        <v>0.9982868062978894</v>
+        <v>0.9960465209814735</v>
       </c>
       <c r="AM29" t="n" s="83">
-        <v>0.9999987242562152</v>
+        <v>1.0</v>
       </c>
       <c r="AN29" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO29" t="n" s="83">
-        <v>0.9911231210102833</v>
+        <v>1.0</v>
       </c>
       <c r="AP29" t="n" s="83">
         <v>1.0</v>
@@ -4867,28 +4867,28 @@
         <v>0.5</v>
       </c>
       <c r="AI30" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9988289146221508</v>
       </c>
       <c r="AJ30" t="n" s="83">
-        <v>0.9074129222781414</v>
+        <v>0.9383107166319116</v>
       </c>
       <c r="AK30" t="n" s="83">
-        <v>0.12661493886450953</v>
+        <v>0.3580154930869824</v>
       </c>
       <c r="AL30" t="n" s="83">
-        <v>0.9347469238292465</v>
+        <v>0.947384050892761</v>
       </c>
       <c r="AM30" t="n" s="83">
-        <v>0.3806329364591275</v>
+        <v>0.7096513806662211</v>
       </c>
       <c r="AN30" t="n" s="83">
-        <v>1.7643255916747912E-10</v>
+        <v>0.9999608509607909</v>
       </c>
       <c r="AO30" t="n" s="83">
-        <v>0.6523062942436713</v>
+        <v>0.6900105537080569</v>
       </c>
       <c r="AP30" t="n" s="83">
-        <v>2.3468131431798405E-8</v>
+        <v>6.352151249946083E-8</v>
       </c>
       <c r="AQ30" t="n" s="83">
         <v>2.3021300241567363E-36</v>
@@ -4989,25 +4989,25 @@
         <v>0.5</v>
       </c>
       <c r="AI31" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ31" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK31" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL31" t="n" s="83">
-        <v>0.9999832523071457</v>
+        <v>0.9999292374119777</v>
       </c>
       <c r="AM31" t="n" s="83">
-        <v>0.9999999999999996</v>
+        <v>1.0</v>
       </c>
       <c r="AN31" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO31" t="n" s="83">
-        <v>0.9999998539139474</v>
+        <v>1.0</v>
       </c>
       <c r="AP31" t="n" s="83">
         <v>1.0</v>
@@ -5111,28 +5111,28 @@
         <v>0.5</v>
       </c>
       <c r="AI32" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9988289146221508</v>
       </c>
       <c r="AJ32" t="n" s="83">
-        <v>0.8987325046910183</v>
+        <v>0.9323110056753068</v>
       </c>
       <c r="AK32" t="n" s="83">
-        <v>0.025412569209433557</v>
+        <v>0.06683382683821781</v>
       </c>
       <c r="AL32" t="n" s="83">
-        <v>0.9307584856780335</v>
+        <v>0.9441218528246201</v>
       </c>
       <c r="AM32" t="n" s="83">
-        <v>0.2166374433559105</v>
+        <v>0.523777978383254</v>
       </c>
       <c r="AN32" t="n" s="83">
-        <v>2.740372403274988E-12</v>
+        <v>0.9969448181611544</v>
       </c>
       <c r="AO32" t="n" s="83">
-        <v>0.6523062639462035</v>
+        <v>0.6900105346591806</v>
       </c>
       <c r="AP32" t="n" s="83">
-        <v>2.7188961678192453E-9</v>
+        <v>7.359273725175092E-9</v>
       </c>
       <c r="AQ32" t="n" s="83">
         <v>6.704201331547735E-39</v>
@@ -5233,28 +5233,28 @@
         <v>0.5</v>
       </c>
       <c r="AI33" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ33" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK33" t="n" s="83">
-        <v>0.07541813561346608</v>
+        <v>0.1378323296798708</v>
       </c>
       <c r="AL33" t="n" s="83">
-        <v>0.9836875112577306</v>
+        <v>0.9878665993448128</v>
       </c>
       <c r="AM33" t="n" s="83">
-        <v>0.8980772299438537</v>
+        <v>0.9805180153320261</v>
       </c>
       <c r="AN33" t="n" s="83">
-        <v>1.6725824871100036E-9</v>
+        <v>0.03780008170933085</v>
       </c>
       <c r="AO33" t="n" s="83">
-        <v>0.8660762251141307</v>
+        <v>0.9191865767349978</v>
       </c>
       <c r="AP33" t="n" s="83">
-        <v>6.145054538843331E-6</v>
+        <v>0.9928639601452801</v>
       </c>
       <c r="AQ33" t="n" s="83">
         <v>2.0533755640502E-34</v>
@@ -5355,28 +5355,28 @@
         <v>0.5</v>
       </c>
       <c r="AI34" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ34" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK34" t="n" s="83">
-        <v>0.0754181349899714</v>
+        <v>0.13783232897149583</v>
       </c>
       <c r="AL34" t="n" s="83">
-        <v>0.9765372268261889</v>
+        <v>0.9825155830315134</v>
       </c>
       <c r="AM34" t="n" s="83">
-        <v>0.8980771127548363</v>
+        <v>0.9805179990278212</v>
       </c>
       <c r="AN34" t="n" s="83">
-        <v>5.854038711249399E-10</v>
+        <v>0.013563279085763193</v>
       </c>
       <c r="AO34" t="n" s="83">
-        <v>0.7300873886108452</v>
+        <v>0.772482979257929</v>
       </c>
       <c r="AP34" t="n" s="83">
-        <v>1.7509015977300392E-7</v>
+        <v>6.156032875184385E-7</v>
       </c>
       <c r="AQ34" t="n" s="83">
         <v>1.4658832734971673E-37</v>
@@ -5477,28 +5477,28 @@
         <v>0.5</v>
       </c>
       <c r="AI35" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ35" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK35" t="n" s="83">
-        <v>0.07541813561346608</v>
+        <v>0.1378323296798708</v>
       </c>
       <c r="AL35" t="n" s="83">
-        <v>0.9836875112577306</v>
+        <v>0.9878665993448128</v>
       </c>
       <c r="AM35" t="n" s="83">
-        <v>0.8980772299438537</v>
+        <v>0.9805180153320261</v>
       </c>
       <c r="AN35" t="n" s="83">
-        <v>1.6725824871100036E-9</v>
+        <v>0.03780008170933085</v>
       </c>
       <c r="AO35" t="n" s="83">
-        <v>0.8660762251141307</v>
+        <v>0.9191865767349978</v>
       </c>
       <c r="AP35" t="n" s="83">
-        <v>6.145054538843331E-6</v>
+        <v>0.9928639601452801</v>
       </c>
       <c r="AQ35" t="n" s="83">
         <v>2.0533755640502E-34</v>
@@ -5599,28 +5599,28 @@
         <v>0.5</v>
       </c>
       <c r="AI36" t="n" s="83">
-        <v>0.9991103295372367</v>
+        <v>0.9991560784779769</v>
       </c>
       <c r="AJ36" t="n" s="83">
-        <v>0.9793089166228728</v>
+        <v>0.9865689917862578</v>
       </c>
       <c r="AK36" t="n" s="83">
-        <v>0.6876417740620906</v>
+        <v>0.922221447307234</v>
       </c>
       <c r="AL36" t="n" s="83">
-        <v>0.9973771382926307</v>
+        <v>0.9981270372616223</v>
       </c>
       <c r="AM36" t="n" s="83">
-        <v>0.9791929167429633</v>
+        <v>0.9968317086232488</v>
       </c>
       <c r="AN36" t="n" s="83">
-        <v>0.21291836821245083</v>
+        <v>1.0</v>
       </c>
       <c r="AO36" t="n" s="83">
-        <v>0.9793994234682715</v>
+        <v>0.993981372044012</v>
       </c>
       <c r="AP36" t="n" s="83">
-        <v>0.9132381103977213</v>
+        <v>1.0</v>
       </c>
       <c r="AQ36" t="n" s="83">
         <v>2.631844059530539E-13</v>
@@ -5721,28 +5721,28 @@
         <v>0.5</v>
       </c>
       <c r="AI37" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ37" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK37" t="n" s="83">
-        <v>0.07541813549356326</v>
+        <v>0.13783232954364485</v>
       </c>
       <c r="AL37" t="n" s="83">
-        <v>0.9839786572894015</v>
+        <v>0.9880840603561512</v>
       </c>
       <c r="AM37" t="n" s="83">
-        <v>0.8980772185031288</v>
+        <v>0.9805180137403072</v>
       </c>
       <c r="AN37" t="n" s="83">
-        <v>1.4635096765272338E-9</v>
+        <v>0.03323209347676371</v>
       </c>
       <c r="AO37" t="n" s="83">
-        <v>0.867810193633498</v>
+        <v>0.920280261830728</v>
       </c>
       <c r="AP37" t="n" s="83">
-        <v>5.574133662959207E-6</v>
+        <v>0.992078958065397</v>
       </c>
       <c r="AQ37" t="n" s="83">
         <v>1.2991054020890683E-34</v>
@@ -5843,28 +5843,28 @@
         <v>0.5</v>
       </c>
       <c r="AI38" t="n" s="83">
-        <v>0.9989177443749853</v>
+        <v>0.9989733863204286</v>
       </c>
       <c r="AJ38" t="n" s="83">
-        <v>0.9070789731786727</v>
+        <v>0.9380806070607488</v>
       </c>
       <c r="AK38" t="n" s="83">
-        <v>0.019984954677613714</v>
+        <v>0.03843084143520047</v>
       </c>
       <c r="AL38" t="n" s="83">
-        <v>0.9678731231818247</v>
+        <v>0.9752272136877697</v>
       </c>
       <c r="AM38" t="n" s="83">
-        <v>0.5322606046754733</v>
+        <v>0.8448873680338381</v>
       </c>
       <c r="AN38" t="n" s="83">
-        <v>3.476212878469919E-12</v>
+        <v>7.209847169916013E-5</v>
       </c>
       <c r="AO38" t="n" s="83">
-        <v>0.8493105854605634</v>
+        <v>0.9062964197719305</v>
       </c>
       <c r="AP38" t="n" s="83">
-        <v>1.9627213916082556E-7</v>
+        <v>0.7969298263362011</v>
       </c>
       <c r="AQ38" t="n" s="83">
         <v>7.261544626463818E-38</v>
@@ -5965,25 +5965,25 @@
         <v>0.5</v>
       </c>
       <c r="AI39" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ39" t="n" s="83">
-        <v>0.9999866121484826</v>
+        <v>0.9999359251171547</v>
       </c>
       <c r="AK39" t="n" s="83">
-        <v>0.9999999987621196</v>
+        <v>1.0</v>
       </c>
       <c r="AL39" t="n" s="83">
-        <v>0.9999659368345347</v>
+        <v>0.9998560838702113</v>
       </c>
       <c r="AM39" t="n" s="83">
-        <v>0.999999999999573</v>
+        <v>1.0</v>
       </c>
       <c r="AN39" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO39" t="n" s="83">
-        <v>0.9999994278489777</v>
+        <v>1.0</v>
       </c>
       <c r="AP39" t="n" s="83">
         <v>1.0</v>
@@ -6087,28 +6087,28 @@
         <v>0.5</v>
       </c>
       <c r="AI40" t="n" s="83">
-        <v>0.7615850757590413</v>
+        <v>0.7710459687810896</v>
       </c>
       <c r="AJ40" t="n" s="83">
-        <v>0.10113948525936915</v>
+        <v>0.1363651309905282</v>
       </c>
       <c r="AK40" t="n" s="83">
-        <v>7.107617348924314E-4</v>
+        <v>0.0025261720368593473</v>
       </c>
       <c r="AL40" t="n" s="83">
-        <v>0.0850011765623238</v>
+        <v>0.11178261162206608</v>
       </c>
       <c r="AM40" t="n" s="83">
-        <v>1.8033128666795828E-6</v>
+        <v>7.0567503676874096E-6</v>
       </c>
       <c r="AN40" t="n" s="83">
-        <v>3.34950693638483E-20</v>
+        <v>3.5908531514736485E-13</v>
       </c>
       <c r="AO40" t="n" s="83">
-        <v>3.118114002136432E-5</v>
+        <v>3.9294702501207746E-5</v>
       </c>
       <c r="AP40" t="n" s="83">
-        <v>5.21928487260433E-22</v>
+        <v>1.3980215344029998E-21</v>
       </c>
       <c r="AQ40" t="n" s="83">
         <v>1.121735973981497E-53</v>
@@ -6209,28 +6209,28 @@
         <v>0.5</v>
       </c>
       <c r="AI41" t="n" s="83">
-        <v>0.999006305936356</v>
+        <v>0.9990573989679111</v>
       </c>
       <c r="AJ41" t="n" s="83">
-        <v>0.9576767689906205</v>
+        <v>0.9713180917605175</v>
       </c>
       <c r="AK41" t="n" s="83">
-        <v>0.13086264263775027</v>
+        <v>0.2228237391610733</v>
       </c>
       <c r="AL41" t="n" s="83">
-        <v>0.9927763656290799</v>
+        <v>0.994834853402433</v>
       </c>
       <c r="AM41" t="n" s="83">
-        <v>0.9532176085820759</v>
+        <v>0.9914913768624616</v>
       </c>
       <c r="AN41" t="n" s="83">
-        <v>2.73171090239185E-8</v>
+        <v>0.39133315193145496</v>
       </c>
       <c r="AO41" t="n" s="83">
-        <v>0.889977094332537</v>
+        <v>0.9361308774796815</v>
       </c>
       <c r="AP41" t="n" s="83">
-        <v>1.857345239153092E-6</v>
+        <v>8.002455674909735E-6</v>
       </c>
       <c r="AQ41" t="n" s="83">
         <v>1.5284192415899508E-34</v>
@@ -6331,28 +6331,28 @@
         <v>0.5</v>
       </c>
       <c r="AI42" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ42" t="n" s="83">
-        <v>0.9439814381568089</v>
+        <v>0.9631710324320358</v>
       </c>
       <c r="AK42" t="n" s="83">
-        <v>0.15700845696071744</v>
+        <v>0.3384384128748147</v>
       </c>
       <c r="AL42" t="n" s="83">
-        <v>0.9836875112577306</v>
+        <v>0.9878665993448128</v>
       </c>
       <c r="AM42" t="n" s="83">
-        <v>0.8980777639408846</v>
+        <v>0.9805180896257748</v>
       </c>
       <c r="AN42" t="n" s="83">
-        <v>1.13458042525168E-7</v>
+        <v>0.9999999430172872</v>
       </c>
       <c r="AO42" t="n" s="83">
-        <v>0.8660768779164872</v>
+        <v>0.9191868554527856</v>
       </c>
       <c r="AP42" t="n" s="83">
-        <v>3.072451747887432E-5</v>
+        <v>0.9985645975578281</v>
       </c>
       <c r="AQ42" t="n" s="83">
         <v>2.1335131130027344E-30</v>
@@ -6453,28 +6453,28 @@
         <v>0.5</v>
       </c>
       <c r="AI43" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9991221140378636</v>
       </c>
       <c r="AJ43" t="n" s="83">
-        <v>0.9810858555481092</v>
+        <v>0.9877302511410424</v>
       </c>
       <c r="AK43" t="n" s="83">
-        <v>0.24601142606806406</v>
+        <v>0.39004637090131455</v>
       </c>
       <c r="AL43" t="n" s="83">
-        <v>0.9950814895289244</v>
+        <v>0.9964739200265905</v>
       </c>
       <c r="AM43" t="n" s="83">
-        <v>0.9832626213731477</v>
+        <v>0.9975134808012177</v>
       </c>
       <c r="AN43" t="n" s="83">
-        <v>3.9854147252889284E-7</v>
+        <v>0.9140113009287065</v>
       </c>
       <c r="AO43" t="n" s="83">
-        <v>0.8813222180208912</v>
+        <v>0.9305987227850674</v>
       </c>
       <c r="AP43" t="n" s="83">
-        <v>1.1466677666372354E-4</v>
+        <v>0.999663501723961</v>
       </c>
       <c r="AQ43" t="n" s="83">
         <v>4.384460207367395E-31</v>
@@ -6575,28 +6575,28 @@
         <v>0.5</v>
       </c>
       <c r="AI44" t="n" s="83">
-        <v>0.5825967006375604</v>
+        <v>0.5953867874863769</v>
       </c>
       <c r="AJ44" t="n" s="83">
-        <v>0.0012288133025817065</v>
+        <v>0.001556709724847345</v>
       </c>
       <c r="AK44" t="n" s="83">
-        <v>1.7013998220604048E-12</v>
+        <v>2.8542106340896702E-12</v>
       </c>
       <c r="AL44" t="n" s="83">
-        <v>6.895480552771871E-4</v>
+        <v>7.711092239315905E-4</v>
       </c>
       <c r="AM44" t="n" s="83">
-        <v>6.206338205636857E-19</v>
+        <v>9.127963666103086E-19</v>
       </c>
       <c r="AN44" t="n" s="83">
-        <v>2.7496353285099376E-49</v>
+        <v>4.5114017340073305E-49</v>
       </c>
       <c r="AO44" t="n" s="83">
-        <v>1.6026776057873426E-10</v>
+        <v>1.7505798994368307E-10</v>
       </c>
       <c r="AP44" t="n" s="83">
-        <v>2.1007579836039155E-44</v>
+        <v>2.81845363109191E-44</v>
       </c>
       <c r="AQ44" t="n" s="83">
         <v>4.7521354302334254E-95</v>
@@ -6697,28 +6697,28 @@
         <v>0.5</v>
       </c>
       <c r="AI45" t="n" s="83">
-        <v>0.852288690535177</v>
+        <v>0.8588174804990142</v>
       </c>
       <c r="AJ45" t="n" s="83">
-        <v>0.18772624292656712</v>
+        <v>0.2454373408994414</v>
       </c>
       <c r="AK45" t="n" s="83">
-        <v>5.49185166983688E-4</v>
+        <v>0.002742982583722911</v>
       </c>
       <c r="AL45" t="n" s="83">
-        <v>0.1458037799758463</v>
+        <v>0.18390612656480687</v>
       </c>
       <c r="AM45" t="n" s="83">
-        <v>1.4925993507164658E-7</v>
+        <v>3.655634613987391E-7</v>
       </c>
       <c r="AN45" t="n" s="83">
-        <v>1.1882299935719774E-23</v>
+        <v>3.954462691024517E-17</v>
       </c>
       <c r="AO45" t="n" s="83">
-        <v>1.7466472156874076E-4</v>
+        <v>3.0328905022497814E-4</v>
       </c>
       <c r="AP45" t="n" s="83">
-        <v>9.753248493557808E-24</v>
+        <v>2.3129139110551333E-23</v>
       </c>
       <c r="AQ45" t="n" s="83">
         <v>1.3423374759254552E-56</v>
@@ -6819,28 +6819,28 @@
         <v>0.5</v>
       </c>
       <c r="AI46" t="n" s="83">
-        <v>0.6853705750715989</v>
+        <v>0.6966511904952137</v>
       </c>
       <c r="AJ46" t="n" s="83">
-        <v>0.04566793876626741</v>
+        <v>0.06068768843060908</v>
       </c>
       <c r="AK46" t="n" s="83">
-        <v>1.94862807915544E-4</v>
+        <v>6.72342919365517E-4</v>
       </c>
       <c r="AL46" t="n" s="83">
-        <v>0.04561282882394601</v>
+        <v>0.060615604594460484</v>
       </c>
       <c r="AM46" t="n" s="83">
-        <v>1.3104507840047902E-7</v>
+        <v>4.947598663402987E-7</v>
       </c>
       <c r="AN46" t="n" s="83">
-        <v>2.271048997650491E-21</v>
+        <v>8.229189100905673E-15</v>
       </c>
       <c r="AO46" t="n" s="83">
-        <v>3.6723588261288262E-6</v>
+        <v>4.609650195469589E-6</v>
       </c>
       <c r="AP46" t="n" s="83">
-        <v>4.8464849813789295E-24</v>
+        <v>1.2576100837985031E-23</v>
       </c>
       <c r="AQ46" t="n" s="83">
         <v>4.7349917575790704E-55</v>
@@ -6941,28 +6941,28 @@
         <v>0.5</v>
       </c>
       <c r="AI47" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9988289146221508</v>
       </c>
       <c r="AJ47" t="n" s="83">
-        <v>0.8983448208260167</v>
+        <v>0.9320421506214364</v>
       </c>
       <c r="AK47" t="n" s="83">
-        <v>0.011290859431024298</v>
+        <v>0.02189144614133825</v>
       </c>
       <c r="AL47" t="n" s="83">
-        <v>0.9307584856780335</v>
+        <v>0.9441218528246201</v>
       </c>
       <c r="AM47" t="n" s="83">
-        <v>0.21663743709526972</v>
+        <v>0.5237779722486302</v>
       </c>
       <c r="AN47" t="n" s="83">
-        <v>4.013833580737733E-14</v>
+        <v>7.257747874035295E-7</v>
       </c>
       <c r="AO47" t="n" s="83">
-        <v>0.652306255731659</v>
+        <v>0.6900105294944638</v>
       </c>
       <c r="AP47" t="n" s="83">
-        <v>5.437792347466324E-10</v>
+        <v>1.4718547537004434E-9</v>
       </c>
       <c r="AQ47" t="n" s="83">
         <v>6.452374430176985E-43</v>
@@ -7063,28 +7063,28 @@
         <v>0.5</v>
       </c>
       <c r="AI48" t="n" s="83">
-        <v>0.8500986151475927</v>
+        <v>0.8567079380802765</v>
       </c>
       <c r="AJ48" t="n" s="83">
-        <v>0.19669251020622816</v>
+        <v>0.25441937535119075</v>
       </c>
       <c r="AK48" t="n" s="83">
-        <v>2.2858615414079994E-5</v>
+        <v>4.1151706643993415E-5</v>
       </c>
       <c r="AL48" t="n" s="83">
-        <v>0.10971293329950056</v>
+        <v>0.1303706314026786</v>
       </c>
       <c r="AM48" t="n" s="83">
-        <v>3.161710058599298E-6</v>
+        <v>9.67953272312245E-6</v>
       </c>
       <c r="AN48" t="n" s="83">
-        <v>1.1135406103047937E-23</v>
+        <v>1.6577693432928848E-16</v>
       </c>
       <c r="AO48" t="n" s="83">
-        <v>9.752668013316614E-4</v>
+        <v>0.001128805683714101</v>
       </c>
       <c r="AP48" t="n" s="83">
-        <v>1.7637965076207936E-20</v>
+        <v>3.9306649664147655E-20</v>
       </c>
       <c r="AQ48" t="n" s="83">
         <v>5.829589821522494E-57</v>
@@ -7185,28 +7185,28 @@
         <v>0.5</v>
       </c>
       <c r="AI49" t="n" s="83">
-        <v>0.9990073756964236</v>
+        <v>0.999058413775684</v>
       </c>
       <c r="AJ49" t="n" s="83">
-        <v>0.9399809940375758</v>
+        <v>0.96048360539935</v>
       </c>
       <c r="AK49" t="n" s="83">
-        <v>0.06760485684941663</v>
+        <v>0.12442312898349837</v>
       </c>
       <c r="AL49" t="n" s="83">
-        <v>0.976332310092944</v>
+        <v>0.9823788751603242</v>
       </c>
       <c r="AM49" t="n" s="83">
-        <v>0.8903429888887523</v>
+        <v>0.9789183093530307</v>
       </c>
       <c r="AN49" t="n" s="83">
-        <v>3.9779241902467383E-10</v>
+        <v>0.009275591425846375</v>
       </c>
       <c r="AO49" t="n" s="83">
-        <v>0.7338953988795989</v>
+        <v>0.7760798342828594</v>
       </c>
       <c r="AP49" t="n" s="83">
-        <v>1.5130911810335925E-7</v>
+        <v>5.33085273199004E-7</v>
       </c>
       <c r="AQ49" t="n" s="83">
         <v>9.006738616644905E-38</v>
@@ -7307,25 +7307,25 @@
         <v>0.5</v>
       </c>
       <c r="AI50" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ50" t="n" s="83">
-        <v>0.9999827953445111</v>
+        <v>0.9999176589049187</v>
       </c>
       <c r="AK50" t="n" s="83">
-        <v>0.9999364654944327</v>
+        <v>1.0</v>
       </c>
       <c r="AL50" t="n" s="83">
-        <v>0.9998717594429295</v>
+        <v>0.999386501478298</v>
       </c>
       <c r="AM50" t="n" s="83">
-        <v>0.9999910560071051</v>
+        <v>1.0</v>
       </c>
       <c r="AN50" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO50" t="n" s="83">
-        <v>0.9833753180847122</v>
+        <v>1.0</v>
       </c>
       <c r="AP50" t="n" s="83">
         <v>1.0</v>
@@ -7429,25 +7429,25 @@
         <v>0.5</v>
       </c>
       <c r="AI51" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ51" t="n" s="83">
-        <v>0.9999936600525205</v>
+        <v>0.9999696559054562</v>
       </c>
       <c r="AK51" t="n" s="83">
-        <v>0.99999867490031</v>
+        <v>1.0</v>
       </c>
       <c r="AL51" t="n" s="83">
-        <v>0.9999883603959002</v>
+        <v>0.9999442919422401</v>
       </c>
       <c r="AM51" t="n" s="83">
-        <v>0.9999999994020954</v>
+        <v>1.0</v>
       </c>
       <c r="AN51" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO51" t="n" s="83">
-        <v>0.999952927336288</v>
+        <v>1.0</v>
       </c>
       <c r="AP51" t="n" s="83">
         <v>1.0</v>
@@ -7551,28 +7551,28 @@
         <v>0.5</v>
       </c>
       <c r="AI52" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9992586000660587</v>
       </c>
       <c r="AJ52" t="n" s="83">
-        <v>0.9998007380944234</v>
+        <v>0.9998715977335384</v>
       </c>
       <c r="AK52" t="n" s="83">
-        <v>0.9224148947433747</v>
+        <v>0.9701591295636491</v>
       </c>
       <c r="AL52" t="n" s="83">
-        <v>0.999919287680545</v>
+        <v>0.9999460162681404</v>
       </c>
       <c r="AM52" t="n" s="83">
-        <v>0.9996668041500031</v>
+        <v>0.9999642643324795</v>
       </c>
       <c r="AN52" t="n" s="83">
-        <v>0.641606968771728</v>
+        <v>0.9999999999999976</v>
       </c>
       <c r="AO52" t="n" s="83">
-        <v>0.9844909292284908</v>
+        <v>0.9956258172117005</v>
       </c>
       <c r="AP52" t="n" s="83">
-        <v>0.9854879932509297</v>
+        <v>1.0</v>
       </c>
       <c r="AQ52" t="n" s="83">
         <v>1.1502840223021237E-13</v>
@@ -7673,25 +7673,25 @@
         <v>0.5</v>
       </c>
       <c r="AI53" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ53" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK53" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL53" t="n" s="83">
-        <v>0.9999744279750036</v>
+        <v>0.9998919557943996</v>
       </c>
       <c r="AM53" t="n" s="83">
-        <v>0.9999999999999984</v>
+        <v>1.0</v>
       </c>
       <c r="AN53" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO53" t="n" s="83">
-        <v>0.9999987328523009</v>
+        <v>1.0</v>
       </c>
       <c r="AP53" t="n" s="83">
         <v>1.0</v>
@@ -7795,28 +7795,28 @@
         <v>0.5</v>
       </c>
       <c r="AI54" t="n" s="83">
-        <v>0.9992488414630909</v>
+        <v>0.9992874728754778</v>
       </c>
       <c r="AJ54" t="n" s="83">
-        <v>0.9997685417919141</v>
+        <v>0.9998508490683815</v>
       </c>
       <c r="AK54" t="n" s="83">
-        <v>0.9748531198585203</v>
+        <v>0.9950612799821241</v>
       </c>
       <c r="AL54" t="n" s="83">
-        <v>0.9997831729327564</v>
+        <v>0.9998554452319804</v>
       </c>
       <c r="AM54" t="n" s="83">
-        <v>0.9995447572708445</v>
+        <v>0.9999515438610941</v>
       </c>
       <c r="AN54" t="n" s="83">
-        <v>0.9934884952557151</v>
+        <v>1.0</v>
       </c>
       <c r="AO54" t="n" s="83">
-        <v>0.9151491758886678</v>
+        <v>0.9534811727460352</v>
       </c>
       <c r="AP54" t="n" s="83">
-        <v>0.4273539190241322</v>
+        <v>0.9999999601591433</v>
       </c>
       <c r="AQ54" t="n" s="83">
         <v>1.692933039143313E-13</v>
@@ -7917,28 +7917,28 @@
         <v>0.5</v>
       </c>
       <c r="AI55" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ55" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999988177650597</v>
       </c>
       <c r="AK55" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>0.9999999999922596</v>
       </c>
       <c r="AL55" t="n" s="83">
-        <v>0.9993744113189219</v>
+        <v>0.9995365738711016</v>
       </c>
       <c r="AM55" t="n" s="83">
-        <v>0.9999999951354414</v>
+        <v>0.9999999981342332</v>
       </c>
       <c r="AN55" t="n" s="83">
-        <v>0.9999999995857503</v>
+        <v>1.0</v>
       </c>
       <c r="AO55" t="n" s="83">
-        <v>0.9804205571019377</v>
+        <v>0.9772906224640616</v>
       </c>
       <c r="AP55" t="n" s="83">
-        <v>0.9918645376684081</v>
+        <v>0.9976725598593037</v>
       </c>
       <c r="AQ55" t="n" s="83">
         <v>0.44683149221674895</v>
@@ -8039,28 +8039,28 @@
         <v>0.5</v>
       </c>
       <c r="AI56" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9991221140378636</v>
       </c>
       <c r="AJ56" t="n" s="83">
-        <v>0.9988790077598008</v>
+        <v>0.9992774075489064</v>
       </c>
       <c r="AK56" t="n" s="83">
-        <v>0.999796995679348</v>
+        <v>0.9999857435722815</v>
       </c>
       <c r="AL56" t="n" s="83">
-        <v>0.9975019536322183</v>
+        <v>0.9982103830189125</v>
       </c>
       <c r="AM56" t="n" s="83">
-        <v>0.9996570117348362</v>
+        <v>0.9999216444491114</v>
       </c>
       <c r="AN56" t="n" s="83">
-        <v>0.9999969766519622</v>
+        <v>1.0</v>
       </c>
       <c r="AO56" t="n" s="83">
-        <v>0.9019341658613231</v>
+        <v>0.9395437213060891</v>
       </c>
       <c r="AP56" t="n" s="83">
-        <v>0.8394330623753135</v>
+        <v>0.9999999926160889</v>
       </c>
       <c r="AQ56" t="n" s="83">
         <v>4.148562433703532E-6</v>
@@ -8161,25 +8161,25 @@
         <v>0.5</v>
       </c>
       <c r="AI57" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ57" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK57" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL57" t="n" s="83">
-        <v>0.9999209791348291</v>
+        <v>0.9996661869717071</v>
       </c>
       <c r="AM57" t="n" s="83">
-        <v>0.9999999999999412</v>
+        <v>1.0</v>
       </c>
       <c r="AN57" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO57" t="n" s="83">
-        <v>0.9993850664496642</v>
+        <v>1.0</v>
       </c>
       <c r="AP57" t="n" s="83">
         <v>1.0</v>
@@ -8283,28 +8283,28 @@
         <v>0.5</v>
       </c>
       <c r="AI58" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9992586000660587</v>
       </c>
       <c r="AJ58" t="n" s="83">
-        <v>0.9999514996552895</v>
+        <v>0.9999687485661437</v>
       </c>
       <c r="AK58" t="n" s="83">
-        <v>0.9999948809293138</v>
+        <v>0.9999992758687725</v>
       </c>
       <c r="AL58" t="n" s="83">
-        <v>0.999919287680545</v>
+        <v>0.9999460162681404</v>
       </c>
       <c r="AM58" t="n" s="83">
-        <v>0.9999999884542137</v>
+        <v>0.9999999973642457</v>
       </c>
       <c r="AN58" t="n" s="83">
-        <v>0.9999998845609451</v>
+        <v>1.0</v>
       </c>
       <c r="AO58" t="n" s="83">
-        <v>0.9996802976111755</v>
+        <v>0.9998727618408115</v>
       </c>
       <c r="AP58" t="n" s="83">
-        <v>0.9999631903679704</v>
+        <v>1.0</v>
       </c>
       <c r="AQ58" t="n" s="83">
         <v>0.13427694845683455</v>
@@ -8405,25 +8405,25 @@
         <v>0.5</v>
       </c>
       <c r="AI59" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ59" t="n" s="83">
-        <v>0.999994791587739</v>
+        <v>0.9999750715235917</v>
       </c>
       <c r="AK59" t="n" s="83">
-        <v>0.9999989172418282</v>
+        <v>1.0</v>
       </c>
       <c r="AL59" t="n" s="83">
-        <v>0.9999634386555672</v>
+        <v>0.9998455303631983</v>
       </c>
       <c r="AM59" t="n" s="83">
-        <v>0.999999979338035</v>
+        <v>1.0</v>
       </c>
       <c r="AN59" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO59" t="n" s="83">
-        <v>0.9990674936986128</v>
+        <v>1.0</v>
       </c>
       <c r="AP59" t="n" s="83">
         <v>1.0</v>
@@ -8527,25 +8527,25 @@
         <v>0.5</v>
       </c>
       <c r="AI60" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ60" t="n" s="83">
-        <v>0.9999809481281149</v>
+        <v>0.999908818806388</v>
       </c>
       <c r="AK60" t="n" s="83">
-        <v>0.9999998688465175</v>
+        <v>1.0</v>
       </c>
       <c r="AL60" t="n" s="83">
-        <v>0.9998807063141945</v>
+        <v>0.9994961252871444</v>
       </c>
       <c r="AM60" t="n" s="83">
-        <v>0.9999999867296046</v>
+        <v>1.0</v>
       </c>
       <c r="AN60" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO60" t="n" s="83">
-        <v>0.9946065349453047</v>
+        <v>1.0</v>
       </c>
       <c r="AP60" t="n" s="83">
         <v>1.0</v>
@@ -8649,25 +8649,25 @@
         <v>0.5</v>
       </c>
       <c r="AI61" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9988625441701168</v>
       </c>
       <c r="AJ61" t="n" s="83">
-        <v>0.9999986664649917</v>
+        <v>0.9999936173478504</v>
       </c>
       <c r="AK61" t="n" s="83">
-        <v>0.999999999959948</v>
+        <v>1.0</v>
       </c>
       <c r="AL61" t="n" s="83">
-        <v>0.9998322282003985</v>
+        <v>0.9994416955179227</v>
       </c>
       <c r="AM61" t="n" s="83">
-        <v>0.9999999999861159</v>
+        <v>1.0</v>
       </c>
       <c r="AN61" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO61" t="n" s="83">
-        <v>0.9998161185504492</v>
+        <v>1.0</v>
       </c>
       <c r="AP61" t="n" s="83">
         <v>1.0</v>
@@ -8771,25 +8771,25 @@
         <v>0.5</v>
       </c>
       <c r="AI62" t="n" s="83">
-        <v>0.9991384966975401</v>
+        <v>0.9989411524322583</v>
       </c>
       <c r="AJ62" t="n" s="83">
-        <v>0.9999492529692122</v>
+        <v>0.9997849546813367</v>
       </c>
       <c r="AK62" t="n" s="83">
-        <v>0.9999968520250963</v>
+        <v>1.0</v>
       </c>
       <c r="AL62" t="n" s="83">
-        <v>0.9999246801859794</v>
+        <v>0.9996818177677065</v>
       </c>
       <c r="AM62" t="n" s="83">
-        <v>0.9999996395454436</v>
+        <v>1.0</v>
       </c>
       <c r="AN62" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO62" t="n" s="83">
-        <v>0.9986320290636603</v>
+        <v>1.0</v>
       </c>
       <c r="AP62" t="n" s="83">
         <v>1.0</v>
@@ -8893,28 +8893,28 @@
         <v>0.5</v>
       </c>
       <c r="AI63" t="n" s="83">
-        <v>0.987863816656439</v>
+        <v>0.988481220157009</v>
       </c>
       <c r="AJ63" t="n" s="83">
-        <v>0.6780030012415458</v>
+        <v>0.7595334616821736</v>
       </c>
       <c r="AK63" t="n" s="83">
-        <v>0.00501335539017693</v>
+        <v>0.013301823097849993</v>
       </c>
       <c r="AL63" t="n" s="83">
-        <v>0.5172128488402249</v>
+        <v>0.5738462355314451</v>
       </c>
       <c r="AM63" t="n" s="83">
-        <v>0.010841615567494897</v>
+        <v>0.04073676606559976</v>
       </c>
       <c r="AN63" t="n" s="83">
-        <v>6.403447438979856E-15</v>
+        <v>0.4291986803278501</v>
       </c>
       <c r="AO63" t="n" s="83">
-        <v>0.10204939668665697</v>
+        <v>0.11881691141468084</v>
       </c>
       <c r="AP63" t="n" s="83">
-        <v>1.1780146133478306E-12</v>
+        <v>3.1216810333014286E-12</v>
       </c>
       <c r="AQ63" t="n" s="83">
         <v>9.723919110083518E-43</v>
@@ -9015,28 +9015,28 @@
         <v>0.5</v>
       </c>
       <c r="AI64" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9992586000660587</v>
       </c>
       <c r="AJ64" t="n" s="83">
-        <v>0.9996535416535808</v>
+        <v>0.9997767342133144</v>
       </c>
       <c r="AK64" t="n" s="83">
-        <v>0.7024552726329008</v>
+        <v>0.7675430737912123</v>
       </c>
       <c r="AL64" t="n" s="83">
-        <v>0.9999614742744677</v>
+        <v>0.9999742327640475</v>
       </c>
       <c r="AM64" t="n" s="83">
-        <v>0.9997637676789621</v>
+        <v>0.9999722277612744</v>
       </c>
       <c r="AN64" t="n" s="83">
-        <v>0.0067971222466370294</v>
+        <v>0.03403136480386842</v>
       </c>
       <c r="AO64" t="n" s="83">
-        <v>0.9979192652488539</v>
+        <v>0.9996740437956458</v>
       </c>
       <c r="AP64" t="n" s="83">
-        <v>0.9996558290240879</v>
+        <v>1.0</v>
       </c>
       <c r="AQ64" t="n" s="83">
         <v>4.823955781714656E-15</v>
@@ -9137,25 +9137,25 @@
         <v>0.5</v>
       </c>
       <c r="AI65" t="n" s="83">
-        <v>0.9990739168110178</v>
+        <v>0.9988617961056364</v>
       </c>
       <c r="AJ65" t="n" s="83">
-        <v>0.9986485615680448</v>
+        <v>0.9942836652107085</v>
       </c>
       <c r="AK65" t="n" s="83">
-        <v>0.998497598568461</v>
+        <v>1.0</v>
       </c>
       <c r="AL65" t="n" s="83">
-        <v>0.9993241597667982</v>
+        <v>0.9974699187867525</v>
       </c>
       <c r="AM65" t="n" s="83">
-        <v>0.999577635108817</v>
+        <v>1.0</v>
       </c>
       <c r="AN65" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO65" t="n" s="83">
-        <v>0.9830151353096767</v>
+        <v>1.0</v>
       </c>
       <c r="AP65" t="n" s="83">
         <v>1.0</v>
@@ -9259,28 +9259,28 @@
         <v>0.5</v>
       </c>
       <c r="AI66" t="n" s="83">
-        <v>0.857288604307878</v>
+        <v>0.8636316750156766</v>
       </c>
       <c r="AJ66" t="n" s="83">
-        <v>0.21023971237932426</v>
+        <v>0.2790075575708584</v>
       </c>
       <c r="AK66" t="n" s="83">
-        <v>0.003456367110745484</v>
+        <v>0.017640704475866492</v>
       </c>
       <c r="AL66" t="n" s="83">
-        <v>0.15777797779971173</v>
+        <v>0.20281696326322682</v>
       </c>
       <c r="AM66" t="n" s="83">
-        <v>6.81834203851803E-7</v>
+        <v>2.3704370397166365E-6</v>
       </c>
       <c r="AN66" t="n" s="83">
-        <v>4.43307225113981E-22</v>
+        <v>1.5542505828993087E-16</v>
       </c>
       <c r="AO66" t="n" s="83">
-        <v>1.5245303784674667E-5</v>
+        <v>1.9262370428705128E-5</v>
       </c>
       <c r="AP66" t="n" s="83">
-        <v>3.149954108872318E-24</v>
+        <v>7.885959700137151E-24</v>
       </c>
       <c r="AQ66" t="n" s="83">
         <v>3.542205550905562E-55</v>
@@ -9381,28 +9381,28 @@
         <v>0.5</v>
       </c>
       <c r="AI67" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ67" t="n" s="83">
-        <v>0.9460462837663478</v>
+        <v>0.9645551081043242</v>
       </c>
       <c r="AK67" t="n" s="83">
-        <v>0.29835030713849514</v>
+        <v>0.6207309037883039</v>
       </c>
       <c r="AL67" t="n" s="83">
-        <v>0.9891148631934997</v>
+        <v>0.9919149489069257</v>
       </c>
       <c r="AM67" t="n" s="83">
-        <v>0.8981104294839193</v>
+        <v>0.9805226346950536</v>
       </c>
       <c r="AN67" t="n" s="83">
-        <v>2.0447315774484637E-5</v>
+        <v>1.0</v>
       </c>
       <c r="AO67" t="n" s="83">
-        <v>0.9401232461098255</v>
+        <v>0.9747992313765504</v>
       </c>
       <c r="AP67" t="n" s="83">
-        <v>0.004963421363094724</v>
+        <v>0.9999999999986144</v>
       </c>
       <c r="AQ67" t="n" s="83">
         <v>2.5406151664885096E-23</v>
@@ -9503,28 +9503,28 @@
         <v>0.5</v>
       </c>
       <c r="AI68" t="n" s="83">
-        <v>0.9889693696564325</v>
+        <v>0.9895311264415216</v>
       </c>
       <c r="AJ68" t="n" s="83">
-        <v>0.6889866610348987</v>
+        <v>0.7686848590427059</v>
       </c>
       <c r="AK68" t="n" s="83">
-        <v>0.26100730577686265</v>
+        <v>0.7847375303820309</v>
       </c>
       <c r="AL68" t="n" s="83">
-        <v>0.6144408452513583</v>
+        <v>0.6750269343217603</v>
       </c>
       <c r="AM68" t="n" s="83">
-        <v>0.05723059047459066</v>
+        <v>0.2200092635385232</v>
       </c>
       <c r="AN68" t="n" s="83">
-        <v>2.5726607692474518E-5</v>
+        <v>1.0</v>
       </c>
       <c r="AO68" t="n" s="83">
-        <v>0.2562298528097373</v>
+        <v>0.37080516671628355</v>
       </c>
       <c r="AP68" t="n" s="83">
-        <v>3.4947897300629204E-7</v>
+        <v>0.8710188065292576</v>
       </c>
       <c r="AQ68" t="n" s="83">
         <v>7.07896826165851E-22</v>
@@ -9625,28 +9625,28 @@
         <v>0.5</v>
       </c>
       <c r="AI69" t="n" s="83">
-        <v>0.9909409056580948</v>
+        <v>0.9914031301211035</v>
       </c>
       <c r="AJ69" t="n" s="83">
-        <v>0.6893314396618564</v>
+        <v>0.768970794740734</v>
       </c>
       <c r="AK69" t="n" s="83">
-        <v>0.03435659210687108</v>
+        <v>0.06361091092128415</v>
       </c>
       <c r="AL69" t="n" s="83">
-        <v>0.6118851399169912</v>
+        <v>0.6884190889859787</v>
       </c>
       <c r="AM69" t="n" s="83">
-        <v>0.10461911627174451</v>
+        <v>0.40183743002000394</v>
       </c>
       <c r="AN69" t="n" s="83">
-        <v>1.0681485302547637E-14</v>
+        <v>4.5944807893577095E-14</v>
       </c>
       <c r="AO69" t="n" s="83">
-        <v>0.02147935150111481</v>
+        <v>0.027608192936720077</v>
       </c>
       <c r="AP69" t="n" s="83">
-        <v>7.890955815137945E-14</v>
+        <v>2.811258746905391E-13</v>
       </c>
       <c r="AQ69" t="n" s="83">
         <v>1.3308299052652243E-46</v>
@@ -9747,25 +9747,25 @@
         <v>0.5</v>
       </c>
       <c r="AI70" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ70" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999912182350975</v>
       </c>
       <c r="AK70" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>1.0</v>
       </c>
       <c r="AL70" t="n" s="83">
-        <v>0.9995759674880899</v>
+        <v>0.9987480530251683</v>
       </c>
       <c r="AM70" t="n" s="83">
-        <v>0.9999999986610698</v>
+        <v>1.0</v>
       </c>
       <c r="AN70" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO70" t="n" s="83">
-        <v>0.997740328479794</v>
+        <v>1.0</v>
       </c>
       <c r="AP70" t="n" s="83">
         <v>1.0</v>
@@ -9869,25 +9869,25 @@
         <v>0.5</v>
       </c>
       <c r="AI71" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ71" t="n" s="83">
-        <v>0.9999293312809899</v>
+        <v>0.9996618495441695</v>
       </c>
       <c r="AK71" t="n" s="83">
-        <v>0.9998450377698266</v>
+        <v>1.0</v>
       </c>
       <c r="AL71" t="n" s="83">
-        <v>0.9999435468012974</v>
+        <v>0.9997615036907965</v>
       </c>
       <c r="AM71" t="n" s="83">
-        <v>0.999999811836745</v>
+        <v>1.0</v>
       </c>
       <c r="AN71" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO71" t="n" s="83">
-        <v>0.9998251984152177</v>
+        <v>1.0</v>
       </c>
       <c r="AP71" t="n" s="83">
         <v>1.0</v>
@@ -9991,25 +9991,25 @@
         <v>0.5</v>
       </c>
       <c r="AI72" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9988625441701168</v>
       </c>
       <c r="AJ72" t="n" s="83">
-        <v>0.9826216537898897</v>
+        <v>0.9219573689722044</v>
       </c>
       <c r="AK72" t="n" s="83">
-        <v>0.42311545036740844</v>
+        <v>1.0</v>
       </c>
       <c r="AL72" t="n" s="83">
-        <v>0.9964104585967679</v>
+        <v>0.9881492710934834</v>
       </c>
       <c r="AM72" t="n" s="83">
-        <v>0.9832650065379421</v>
+        <v>1.0</v>
       </c>
       <c r="AN72" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO72" t="n" s="83">
-        <v>0.9434889654949449</v>
+        <v>1.0</v>
       </c>
       <c r="AP72" t="n" s="83">
         <v>1.0</v>
@@ -10113,28 +10113,28 @@
         <v>0.5</v>
       </c>
       <c r="AI73" t="n" s="83">
-        <v>0.9892944798163523</v>
+        <v>0.9898398495329166</v>
       </c>
       <c r="AJ73" t="n" s="83">
-        <v>0.6775141859303936</v>
+        <v>0.7591244034760352</v>
       </c>
       <c r="AK73" t="n" s="83">
-        <v>0.0033447005608139542</v>
+        <v>0.006368907630492176</v>
       </c>
       <c r="AL73" t="n" s="83">
-        <v>0.5294652643686812</v>
+        <v>0.5955450686307343</v>
       </c>
       <c r="AM73" t="n" s="83">
-        <v>0.005705215175073295</v>
+        <v>0.022511480462609677</v>
       </c>
       <c r="AN73" t="n" s="83">
-        <v>7.483537915620657E-19</v>
+        <v>2.499509729254662E-18</v>
       </c>
       <c r="AO73" t="n" s="83">
-        <v>0.036312023993304604</v>
+        <v>0.04417936270247203</v>
       </c>
       <c r="AP73" t="n" s="83">
-        <v>1.2133391533410356E-15</v>
+        <v>3.3321102228820327E-15</v>
       </c>
       <c r="AQ73" t="n" s="83">
         <v>4.615360360735812E-52</v>
@@ -10235,28 +10235,28 @@
         <v>0.5</v>
       </c>
       <c r="AI74" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9988289146221508</v>
       </c>
       <c r="AJ74" t="n" s="83">
-        <v>0.9997715537549691</v>
+        <v>0.9998527901254823</v>
       </c>
       <c r="AK74" t="n" s="83">
-        <v>0.9992217052764925</v>
+        <v>0.9999630885049572</v>
       </c>
       <c r="AL74" t="n" s="83">
-        <v>0.9929128379224529</v>
+        <v>0.9943534081153294</v>
       </c>
       <c r="AM74" t="n" s="83">
-        <v>0.9801679226674843</v>
+        <v>0.9949160991736239</v>
       </c>
       <c r="AN74" t="n" s="83">
-        <v>0.6376233022628182</v>
+        <v>1.0</v>
       </c>
       <c r="AO74" t="n" s="83">
-        <v>0.654422589599803</v>
+        <v>0.6913435203875095</v>
       </c>
       <c r="AP74" t="n" s="83">
-        <v>0.02797954624641204</v>
+        <v>0.07228098430325691</v>
       </c>
       <c r="AQ74" t="n" s="83">
         <v>1.3659996997507443E-16</v>
@@ -10357,28 +10357,28 @@
         <v>0.5</v>
       </c>
       <c r="AI75" t="n" s="83">
-        <v>0.9991824003214459</v>
+        <v>0.9992244460733057</v>
       </c>
       <c r="AJ75" t="n" s="83">
-        <v>0.9944766855023411</v>
+        <v>0.996434081177078</v>
       </c>
       <c r="AK75" t="n" s="83">
-        <v>0.980242871999348</v>
+        <v>0.9981098783669701</v>
       </c>
       <c r="AL75" t="n" s="83">
-        <v>0.985263336532908</v>
+        <v>0.9897894958599796</v>
       </c>
       <c r="AM75" t="n" s="83">
-        <v>0.9808540447791779</v>
+        <v>0.997224588957645</v>
       </c>
       <c r="AN75" t="n" s="83">
-        <v>0.9254246162426071</v>
+        <v>1.0</v>
       </c>
       <c r="AO75" t="n" s="83">
-        <v>0.5379506748611051</v>
+        <v>0.6071710231354527</v>
       </c>
       <c r="AP75" t="n" s="83">
-        <v>6.245299521519128E-4</v>
+        <v>0.002559439856820472</v>
       </c>
       <c r="AQ75" t="n" s="83">
         <v>2.5583413570822093E-17</v>
@@ -10479,28 +10479,28 @@
         <v>0.5</v>
       </c>
       <c r="AI76" t="n" s="83">
-        <v>0.9952910222995766</v>
+        <v>0.9955322907423128</v>
       </c>
       <c r="AJ76" t="n" s="83">
-        <v>0.8487394507844647</v>
+        <v>0.8934983129361652</v>
       </c>
       <c r="AK76" t="n" s="83">
-        <v>0.09270952351297695</v>
+        <v>0.16272451478251654</v>
       </c>
       <c r="AL76" t="n" s="83">
-        <v>0.902092485997909</v>
+        <v>0.9279027517290208</v>
       </c>
       <c r="AM76" t="n" s="83">
-        <v>0.8735212108376265</v>
+        <v>0.9786186947009181</v>
       </c>
       <c r="AN76" t="n" s="83">
-        <v>8.474082729869633E-9</v>
+        <v>0.180612160316154</v>
       </c>
       <c r="AO76" t="n" s="83">
-        <v>0.5564388794185607</v>
+        <v>0.6937342240994937</v>
       </c>
       <c r="AP76" t="n" s="83">
-        <v>1.1415346329082678E-6</v>
+        <v>0.9664883976440489</v>
       </c>
       <c r="AQ76" t="n" s="83">
         <v>4.922609772217173E-34</v>
@@ -10601,28 +10601,28 @@
         <v>0.5</v>
       </c>
       <c r="AI77" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ77" t="n" s="83">
-        <v>0.9438821658525599</v>
+        <v>0.9631044374823134</v>
       </c>
       <c r="AK77" t="n" s="83">
-        <v>0.15494960091791873</v>
+        <v>0.33492139273822363</v>
       </c>
       <c r="AL77" t="n" s="83">
-        <v>0.9765372268261889</v>
+        <v>0.9825155830315134</v>
       </c>
       <c r="AM77" t="n" s="83">
-        <v>0.8980771916822218</v>
+        <v>0.9805180100087828</v>
       </c>
       <c r="AN77" t="n" s="83">
-        <v>5.0327847210546497E-8</v>
+        <v>0.9999998724646808</v>
       </c>
       <c r="AO77" t="n" s="83">
-        <v>0.7300875401694253</v>
+        <v>0.7724830693723257</v>
       </c>
       <c r="AP77" t="n" s="83">
-        <v>1.167266573684311E-6</v>
+        <v>4.104007600293021E-6</v>
       </c>
       <c r="AQ77" t="n" s="83">
         <v>4.443211119983516E-33</v>
@@ -10723,28 +10723,28 @@
         <v>0.5</v>
       </c>
       <c r="AI78" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ78" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK78" t="n" s="83">
-        <v>0.0754181349899714</v>
+        <v>0.13783232897149583</v>
       </c>
       <c r="AL78" t="n" s="83">
-        <v>0.9765372268261889</v>
+        <v>0.9825155830315134</v>
       </c>
       <c r="AM78" t="n" s="83">
-        <v>0.8980771127548363</v>
+        <v>0.9805179990278212</v>
       </c>
       <c r="AN78" t="n" s="83">
-        <v>5.854038711249399E-10</v>
+        <v>0.013563279085763193</v>
       </c>
       <c r="AO78" t="n" s="83">
-        <v>0.7300873886108452</v>
+        <v>0.772482979257929</v>
       </c>
       <c r="AP78" t="n" s="83">
-        <v>1.7509015977300392E-7</v>
+        <v>6.156032875184385E-7</v>
       </c>
       <c r="AQ78" t="n" s="83">
         <v>1.4658832734971673E-37</v>
@@ -10845,25 +10845,25 @@
         <v>0.5</v>
       </c>
       <c r="AI79" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ79" t="n" s="83">
-        <v>0.9999975898290161</v>
+        <v>0.9999884643296152</v>
       </c>
       <c r="AK79" t="n" s="83">
-        <v>0.9999999634678386</v>
+        <v>1.0</v>
       </c>
       <c r="AL79" t="n" s="83">
-        <v>0.9999752815281016</v>
+        <v>0.9998817013135176</v>
       </c>
       <c r="AM79" t="n" s="83">
-        <v>0.9999999974569452</v>
+        <v>1.0</v>
       </c>
       <c r="AN79" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO79" t="n" s="83">
-        <v>0.9938673165781534</v>
+        <v>1.0</v>
       </c>
       <c r="AP79" t="n" s="83">
         <v>1.0</v>
@@ -10967,25 +10967,25 @@
         <v>0.5</v>
       </c>
       <c r="AI80" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ80" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999912182350975</v>
       </c>
       <c r="AK80" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>1.0</v>
       </c>
       <c r="AL80" t="n" s="83">
-        <v>0.9997133626502709</v>
+        <v>0.9991534821357767</v>
       </c>
       <c r="AM80" t="n" s="83">
-        <v>0.9999999996269755</v>
+        <v>1.0</v>
       </c>
       <c r="AN80" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO80" t="n" s="83">
-        <v>0.9997361565408506</v>
+        <v>1.0</v>
       </c>
       <c r="AP80" t="n" s="83">
         <v>1.0</v>
@@ -11089,28 +11089,28 @@
         <v>0.5</v>
       </c>
       <c r="AI81" t="n" s="83">
-        <v>0.9991493793904361</v>
+        <v>0.9991931219178672</v>
       </c>
       <c r="AJ81" t="n" s="83">
-        <v>0.9999564172535871</v>
+        <v>0.9999719172937275</v>
       </c>
       <c r="AK81" t="n" s="83">
-        <v>0.999978668958296</v>
+        <v>0.9999978810543633</v>
       </c>
       <c r="AL81" t="n" s="83">
-        <v>0.9996911263729946</v>
+        <v>0.9997862512819541</v>
       </c>
       <c r="AM81" t="n" s="83">
-        <v>0.9999933646528452</v>
+        <v>0.9999985512472769</v>
       </c>
       <c r="AN81" t="n" s="83">
-        <v>0.9999988218862566</v>
+        <v>1.0</v>
       </c>
       <c r="AO81" t="n" s="83">
-        <v>0.9450441794318463</v>
+        <v>0.9637572450153804</v>
       </c>
       <c r="AP81" t="n" s="83">
-        <v>0.9742297570877685</v>
+        <v>0.9999999991007573</v>
       </c>
       <c r="AQ81" t="n" s="83">
         <v>2.523351031784369E-5</v>
@@ -11211,25 +11211,25 @@
         <v>0.5</v>
       </c>
       <c r="AI82" t="n" s="83">
-        <v>0.9988921685964943</v>
+        <v>0.9986384749298577</v>
       </c>
       <c r="AJ82" t="n" s="83">
-        <v>0.9999489994710343</v>
+        <v>0.999755943840496</v>
       </c>
       <c r="AK82" t="n" s="83">
-        <v>0.9999993526258949</v>
+        <v>1.0</v>
       </c>
       <c r="AL82" t="n" s="83">
-        <v>0.9974788371540041</v>
+        <v>0.9934298869874336</v>
       </c>
       <c r="AM82" t="n" s="83">
-        <v>0.9999813157765584</v>
+        <v>1.0</v>
       </c>
       <c r="AN82" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO82" t="n" s="83">
-        <v>0.966259423372731</v>
+        <v>1.0</v>
       </c>
       <c r="AP82" t="n" s="83">
         <v>1.0</v>
@@ -11333,28 +11333,28 @@
         <v>0.5</v>
       </c>
       <c r="AI83" t="n" s="83">
-        <v>0.9991493793904361</v>
+        <v>0.9991931219064911</v>
       </c>
       <c r="AJ83" t="n" s="83">
-        <v>0.9984880937445636</v>
+        <v>0.9990252883913999</v>
       </c>
       <c r="AK83" t="n" s="83">
-        <v>0.9992373943664389</v>
+        <v>0.9999283358606366</v>
       </c>
       <c r="AL83" t="n" s="83">
-        <v>0.9955211947885253</v>
+        <v>0.9968965612858803</v>
       </c>
       <c r="AM83" t="n" s="83">
-        <v>0.9986877539208423</v>
+        <v>0.9997160631773349</v>
       </c>
       <c r="AN83" t="n" s="83">
-        <v>0.9999710897199614</v>
+        <v>1.0</v>
       </c>
       <c r="AO83" t="n" s="83">
-        <v>0.9145678148050416</v>
+        <v>0.9623924041621992</v>
       </c>
       <c r="AP83" t="n" s="83">
-        <v>0.9360406813716898</v>
+        <v>0.9999999999999974</v>
       </c>
       <c r="AQ83" t="n" s="83">
         <v>6.602339858242662E-6</v>
@@ -11455,25 +11455,25 @@
         <v>0.5</v>
       </c>
       <c r="AI84" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9991519823504463</v>
       </c>
       <c r="AJ84" t="n" s="83">
-        <v>0.999990260531745</v>
+        <v>0.9999533858060138</v>
       </c>
       <c r="AK84" t="n" s="83">
-        <v>0.9998980484414121</v>
+        <v>1.0</v>
       </c>
       <c r="AL84" t="n" s="83">
-        <v>0.999973776860007</v>
+        <v>0.9998745009255523</v>
       </c>
       <c r="AM84" t="n" s="83">
-        <v>0.9999988069468096</v>
+        <v>1.0</v>
       </c>
       <c r="AN84" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO84" t="n" s="83">
-        <v>0.9834302895978223</v>
+        <v>1.0</v>
       </c>
       <c r="AP84" t="n" s="83">
         <v>1.0</v>
@@ -11577,28 +11577,28 @@
         <v>0.5</v>
       </c>
       <c r="AI85" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556630283</v>
       </c>
       <c r="AJ85" t="n" s="83">
-        <v>0.9185211081540053</v>
+        <v>0.945932791276056</v>
       </c>
       <c r="AK85" t="n" s="83">
-        <v>0.16319312820189275</v>
+        <v>0.34876960503010224</v>
       </c>
       <c r="AL85" t="n" s="83">
-        <v>0.9277251810828356</v>
+        <v>0.945446117538972</v>
       </c>
       <c r="AM85" t="n" s="83">
-        <v>0.6387217051209041</v>
+        <v>0.8965649779680248</v>
       </c>
       <c r="AN85" t="n" s="83">
-        <v>1.2093222653696724E-10</v>
+        <v>0.0010893338512956714</v>
       </c>
       <c r="AO85" t="n" s="83">
-        <v>0.4863143614760386</v>
+        <v>0.5430339288976309</v>
       </c>
       <c r="AP85" t="n" s="83">
-        <v>6.6306966024826015E-9</v>
+        <v>2.0946015437628846E-8</v>
       </c>
       <c r="AQ85" t="n" s="83">
         <v>1.978067544289216E-38</v>
@@ -11699,25 +11699,25 @@
         <v>0.5</v>
       </c>
       <c r="AI86" t="n" s="83">
-        <v>0.9898732271897709</v>
+        <v>0.9875798739306365</v>
       </c>
       <c r="AJ86" t="n" s="83">
-        <v>0.9936830095453267</v>
+        <v>0.9737026211545924</v>
       </c>
       <c r="AK86" t="n" s="83">
-        <v>0.9999077542233377</v>
+        <v>1.0</v>
       </c>
       <c r="AL86" t="n" s="83">
-        <v>0.8432899707777651</v>
+        <v>0.6455281875249907</v>
       </c>
       <c r="AM86" t="n" s="83">
-        <v>0.9877212256617067</v>
+        <v>1.0</v>
       </c>
       <c r="AN86" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO86" t="n" s="83">
-        <v>0.3061504850955707</v>
+        <v>1.0</v>
       </c>
       <c r="AP86" t="n" s="83">
         <v>1.0</v>
@@ -11821,28 +11821,28 @@
         <v>0.5</v>
       </c>
       <c r="AI87" t="n" s="83">
-        <v>0.9992488414630909</v>
+        <v>0.9992874728598495</v>
       </c>
       <c r="AJ87" t="n" s="83">
-        <v>0.9987713433937837</v>
+        <v>0.999207976529328</v>
       </c>
       <c r="AK87" t="n" s="83">
-        <v>0.9411210241008752</v>
+        <v>0.984134775710611</v>
       </c>
       <c r="AL87" t="n" s="83">
-        <v>0.9968310697512207</v>
+        <v>0.9978852485872195</v>
       </c>
       <c r="AM87" t="n" s="83">
-        <v>0.997040187358653</v>
+        <v>0.9996474222453045</v>
       </c>
       <c r="AN87" t="n" s="83">
-        <v>0.0065136521381850025</v>
+        <v>0.9999999999931345</v>
       </c>
       <c r="AO87" t="n" s="83">
-        <v>0.575137054745964</v>
+        <v>0.6484864595866409</v>
       </c>
       <c r="AP87" t="n" s="83">
-        <v>8.423446777054117E-5</v>
+        <v>3.926320774221793E-4</v>
       </c>
       <c r="AQ87" t="n" s="83">
         <v>1.4485121489102912E-25</v>
@@ -11943,25 +11943,25 @@
         <v>0.5</v>
       </c>
       <c r="AI88" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9987628592429082</v>
       </c>
       <c r="AJ88" t="n" s="83">
-        <v>0.9999981652120649</v>
+        <v>0.9999912182350975</v>
       </c>
       <c r="AK88" t="n" s="83">
-        <v>0.9999999995758917</v>
+        <v>1.0</v>
       </c>
       <c r="AL88" t="n" s="83">
-        <v>0.9995759674880899</v>
+        <v>0.9987480530251683</v>
       </c>
       <c r="AM88" t="n" s="83">
-        <v>0.9999999986610698</v>
+        <v>1.0</v>
       </c>
       <c r="AN88" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO88" t="n" s="83">
-        <v>0.997740328479794</v>
+        <v>1.0</v>
       </c>
       <c r="AP88" t="n" s="83">
         <v>1.0</v>
@@ -12065,28 +12065,28 @@
         <v>0.5</v>
       </c>
       <c r="AI89" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9992586000556051</v>
       </c>
       <c r="AJ89" t="n" s="83">
-        <v>0.999418580292348</v>
+        <v>0.9996252883058498</v>
       </c>
       <c r="AK89" t="n" s="83">
-        <v>0.9268547150633971</v>
+        <v>0.9720586426503868</v>
       </c>
       <c r="AL89" t="n" s="83">
-        <v>0.9991338567646012</v>
+        <v>0.9994205368459083</v>
       </c>
       <c r="AM89" t="n" s="83">
-        <v>0.998300664578392</v>
+        <v>0.9997967866087536</v>
       </c>
       <c r="AN89" t="n" s="83">
-        <v>0.004096519572143614</v>
+        <v>0.9999838994095518</v>
       </c>
       <c r="AO89" t="n" s="83">
-        <v>0.9046145571022751</v>
+        <v>0.9619491244496269</v>
       </c>
       <c r="AP89" t="n" s="83">
-        <v>0.046250193639643</v>
+        <v>0.9999999999993374</v>
       </c>
       <c r="AQ89" t="n" s="83">
         <v>2.8321426895025983E-22</v>
@@ -12187,25 +12187,25 @@
         <v>0.5</v>
       </c>
       <c r="AI90" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ90" t="n" s="83">
-        <v>0.9998166382468096</v>
+        <v>0.9991229864738413</v>
       </c>
       <c r="AK90" t="n" s="83">
-        <v>0.9999385338362781</v>
+        <v>1.0</v>
       </c>
       <c r="AL90" t="n" s="83">
-        <v>0.9570677610641116</v>
+        <v>0.8406573471079799</v>
       </c>
       <c r="AM90" t="n" s="83">
-        <v>0.9653101214980978</v>
+        <v>1.0</v>
       </c>
       <c r="AN90" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO90" t="n" s="83">
-        <v>0.4771678534257438</v>
+        <v>1.0</v>
       </c>
       <c r="AP90" t="n" s="83">
         <v>1.0</v>
@@ -12309,25 +12309,25 @@
         <v>0.5</v>
       </c>
       <c r="AI91" t="n" s="83">
-        <v>0.9987654520600814</v>
+        <v>0.9984827843506957</v>
       </c>
       <c r="AJ91" t="n" s="83">
-        <v>0.9999962083360194</v>
+        <v>0.9999818522596959</v>
       </c>
       <c r="AK91" t="n" s="83">
-        <v>0.9999999643406988</v>
+        <v>1.0</v>
       </c>
       <c r="AL91" t="n" s="83">
-        <v>0.998316919507106</v>
+        <v>0.9961158590010847</v>
       </c>
       <c r="AM91" t="n" s="83">
-        <v>0.9999987771930935</v>
+        <v>1.0</v>
       </c>
       <c r="AN91" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO91" t="n" s="83">
-        <v>0.9916193030061612</v>
+        <v>1.0</v>
       </c>
       <c r="AP91" t="n" s="83">
         <v>1.0</v>
@@ -12431,28 +12431,28 @@
         <v>0.5</v>
       </c>
       <c r="AI92" t="n" s="83">
-        <v>0.9993100600201867</v>
+        <v>0.9993455448897671</v>
       </c>
       <c r="AJ92" t="n" s="83">
-        <v>0.9995622568786408</v>
+        <v>0.9997178983368469</v>
       </c>
       <c r="AK92" t="n" s="83">
-        <v>0.9973396688874512</v>
+        <v>0.9996529333079247</v>
       </c>
       <c r="AL92" t="n" s="83">
-        <v>0.983178186914151</v>
+        <v>0.9890957052505707</v>
       </c>
       <c r="AM92" t="n" s="83">
-        <v>0.9874322742443433</v>
+        <v>0.9982863675656597</v>
       </c>
       <c r="AN92" t="n" s="83">
-        <v>0.0644556843311822</v>
+        <v>0.9999999999557306</v>
       </c>
       <c r="AO92" t="n" s="83">
-        <v>0.2800190607165498</v>
+        <v>0.43260336803339583</v>
       </c>
       <c r="AP92" t="n" s="83">
-        <v>1.1110172746290665E-4</v>
+        <v>0.9898142666283485</v>
       </c>
       <c r="AQ92" t="n" s="83">
         <v>5.5790597905780674E-21</v>
@@ -12553,25 +12553,25 @@
         <v>0.5</v>
       </c>
       <c r="AI93" t="n" s="83">
-        <v>0.9989549874540834</v>
+        <v>0.998715660825046</v>
       </c>
       <c r="AJ93" t="n" s="83">
-        <v>0.9999760644030731</v>
+        <v>0.9998854476894543</v>
       </c>
       <c r="AK93" t="n" s="83">
-        <v>0.9999839994633144</v>
+        <v>1.0</v>
       </c>
       <c r="AL93" t="n" s="83">
-        <v>0.9924721329027262</v>
+        <v>0.9782184633187945</v>
       </c>
       <c r="AM93" t="n" s="83">
-        <v>0.9951702680350052</v>
+        <v>1.0</v>
       </c>
       <c r="AN93" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO93" t="n" s="83">
-        <v>0.7784321171080184</v>
+        <v>1.0</v>
       </c>
       <c r="AP93" t="n" s="83">
         <v>1.0</v>
@@ -12675,28 +12675,28 @@
         <v>0.5</v>
       </c>
       <c r="AI94" t="n" s="83">
-        <v>0.9669058030551283</v>
+        <v>0.9685554640386276</v>
       </c>
       <c r="AJ94" t="n" s="83">
-        <v>0.4691257518335273</v>
+        <v>0.5605426477439938</v>
       </c>
       <c r="AK94" t="n" s="83">
-        <v>0.016435233804547537</v>
+        <v>0.04186223999941056</v>
       </c>
       <c r="AL94" t="n" s="83">
-        <v>0.3924808401228671</v>
+        <v>0.4655807964599478</v>
       </c>
       <c r="AM94" t="n" s="83">
-        <v>0.008321122330634983</v>
+        <v>0.03733734526605782</v>
       </c>
       <c r="AN94" t="n" s="83">
-        <v>2.240902153851465E-14</v>
+        <v>1.6139322876643406E-7</v>
       </c>
       <c r="AO94" t="n" s="83">
-        <v>0.024072202035054738</v>
+        <v>0.041514763511861334</v>
       </c>
       <c r="AP94" t="n" s="83">
-        <v>4.791996263937024E-13</v>
+        <v>2.7634445741143967E-6</v>
       </c>
       <c r="AQ94" t="n" s="83">
         <v>4.4879958901500624E-42</v>
@@ -12797,28 +12797,28 @@
         <v>0.5</v>
       </c>
       <c r="AI95" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9992586000660587</v>
       </c>
       <c r="AJ95" t="n" s="83">
-        <v>0.9999514996552895</v>
+        <v>0.9999687485661437</v>
       </c>
       <c r="AK95" t="n" s="83">
-        <v>0.9999948809293138</v>
+        <v>0.9999992758687725</v>
       </c>
       <c r="AL95" t="n" s="83">
-        <v>0.999919287680545</v>
+        <v>0.9999460162681404</v>
       </c>
       <c r="AM95" t="n" s="83">
-        <v>0.9999999884542137</v>
+        <v>0.9999999973642457</v>
       </c>
       <c r="AN95" t="n" s="83">
-        <v>0.9999998845609451</v>
+        <v>1.0</v>
       </c>
       <c r="AO95" t="n" s="83">
-        <v>0.9996802976111755</v>
+        <v>0.9998727618408115</v>
       </c>
       <c r="AP95" t="n" s="83">
-        <v>0.9999631903679704</v>
+        <v>1.0</v>
       </c>
       <c r="AQ95" t="n" s="83">
         <v>0.13427694845683455</v>
@@ -12919,28 +12919,28 @@
         <v>0.5</v>
       </c>
       <c r="AI96" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ96" t="n" s="83">
-        <v>0.9438821658525599</v>
+        <v>0.9631044374823134</v>
       </c>
       <c r="AK96" t="n" s="83">
-        <v>0.15494962016290326</v>
+        <v>0.33492141456397184</v>
       </c>
       <c r="AL96" t="n" s="83">
-        <v>0.9839786572894015</v>
+        <v>0.9880840603561512</v>
       </c>
       <c r="AM96" t="n" s="83">
-        <v>0.8980779057118817</v>
+        <v>0.9805181093500746</v>
       </c>
       <c r="AN96" t="n" s="83">
-        <v>1.258196085280212E-7</v>
+        <v>0.9999999489858683</v>
       </c>
       <c r="AO96" t="n" s="83">
-        <v>0.8678110281584852</v>
+        <v>0.9202806176359872</v>
       </c>
       <c r="AP96" t="n" s="83">
-        <v>3.7159717331417445E-5</v>
+        <v>0.9988037897630777</v>
       </c>
       <c r="AQ96" t="n" s="83">
         <v>3.9376880470615084E-30</v>
@@ -13041,28 +13041,28 @@
         <v>0.5</v>
       </c>
       <c r="AI97" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9991221140378636</v>
       </c>
       <c r="AJ97" t="n" s="83">
-        <v>0.9810858555481092</v>
+        <v>0.9877302511410424</v>
       </c>
       <c r="AK97" t="n" s="83">
-        <v>0.2460113940870183</v>
+        <v>0.3900463435552717</v>
       </c>
       <c r="AL97" t="n" s="83">
-        <v>0.9929869822369769</v>
+        <v>0.9949693701453327</v>
       </c>
       <c r="AM97" t="n" s="83">
-        <v>0.9832625095978323</v>
+        <v>0.997513469570477</v>
       </c>
       <c r="AN97" t="n" s="83">
-        <v>1.1956247511409129E-7</v>
+        <v>0.761269884559401</v>
       </c>
       <c r="AO97" t="n" s="83">
-        <v>0.759246170580793</v>
+        <v>0.802500446624334</v>
       </c>
       <c r="AP97" t="n" s="83">
-        <v>2.930227462600291E-6</v>
+        <v>1.1698590110524882E-5</v>
       </c>
       <c r="AQ97" t="n" s="83">
         <v>1.8252163599519083E-34</v>
@@ -13163,28 +13163,28 @@
         <v>0.5</v>
       </c>
       <c r="AI98" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ98" t="n" s="83">
-        <v>0.9438821658525599</v>
+        <v>0.9631044374823134</v>
       </c>
       <c r="AK98" t="n" s="83">
-        <v>0.15494960091791873</v>
+        <v>0.33492139273822363</v>
       </c>
       <c r="AL98" t="n" s="83">
-        <v>0.9765372268261889</v>
+        <v>0.9825155830315134</v>
       </c>
       <c r="AM98" t="n" s="83">
-        <v>0.8980771916822218</v>
+        <v>0.9805180100087828</v>
       </c>
       <c r="AN98" t="n" s="83">
-        <v>5.0327847210546497E-8</v>
+        <v>0.9999998724646808</v>
       </c>
       <c r="AO98" t="n" s="83">
-        <v>0.7300875401694253</v>
+        <v>0.7724830693723257</v>
       </c>
       <c r="AP98" t="n" s="83">
-        <v>1.167266573684311E-6</v>
+        <v>4.104007600293021E-6</v>
       </c>
       <c r="AQ98" t="n" s="83">
         <v>4.443211119983516E-33</v>
@@ -13285,28 +13285,28 @@
         <v>0.5</v>
       </c>
       <c r="AI99" t="n" s="83">
-        <v>0.9992488414630909</v>
+        <v>0.9992874728263602</v>
       </c>
       <c r="AJ99" t="n" s="83">
-        <v>0.9966683408720581</v>
+        <v>0.9978507182160617</v>
       </c>
       <c r="AK99" t="n" s="83">
-        <v>0.9896438177136028</v>
+        <v>0.9986275031690756</v>
       </c>
       <c r="AL99" t="n" s="83">
-        <v>0.9587633215577118</v>
+        <v>0.9721270422763396</v>
       </c>
       <c r="AM99" t="n" s="83">
-        <v>0.9498922738953064</v>
+        <v>0.9915618486913761</v>
       </c>
       <c r="AN99" t="n" s="83">
-        <v>8.451661617052273E-4</v>
+        <v>0.9999999997241277</v>
       </c>
       <c r="AO99" t="n" s="83">
-        <v>0.19592344064100556</v>
+        <v>0.24928766429343613</v>
       </c>
       <c r="AP99" t="n" s="83">
-        <v>5.026728532879398E-7</v>
+        <v>1.886507841095103E-6</v>
       </c>
       <c r="AQ99" t="n" s="83">
         <v>2.4412135260595546E-27</v>
@@ -13407,28 +13407,28 @@
         <v>0.5</v>
       </c>
       <c r="AI100" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ100" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK100" t="n" s="83">
-        <v>0.07541813549356326</v>
+        <v>0.13783232954364485</v>
       </c>
       <c r="AL100" t="n" s="83">
-        <v>0.9839786572894015</v>
+        <v>0.9880840603561512</v>
       </c>
       <c r="AM100" t="n" s="83">
-        <v>0.8980772185031288</v>
+        <v>0.9805180137403072</v>
       </c>
       <c r="AN100" t="n" s="83">
-        <v>1.4635096765272338E-9</v>
+        <v>0.03323209347676371</v>
       </c>
       <c r="AO100" t="n" s="83">
-        <v>0.867810193633498</v>
+        <v>0.920280261830728</v>
       </c>
       <c r="AP100" t="n" s="83">
-        <v>5.574133662959207E-6</v>
+        <v>0.992078958065397</v>
       </c>
       <c r="AQ100" t="n" s="83">
         <v>1.2991054020890683E-34</v>
@@ -13529,28 +13529,28 @@
         <v>0.5</v>
       </c>
       <c r="AI101" t="n" s="83">
-        <v>0.9956537070981696</v>
+        <v>0.9958764700673315</v>
       </c>
       <c r="AJ101" t="n" s="83">
-        <v>0.9869768529357147</v>
+        <v>0.9909521987751557</v>
       </c>
       <c r="AK101" t="n" s="83">
-        <v>0.5814919676193349</v>
+        <v>0.7202383428663178</v>
       </c>
       <c r="AL101" t="n" s="83">
-        <v>0.9946239660952453</v>
+        <v>0.9963979695471302</v>
       </c>
       <c r="AM101" t="n" s="83">
-        <v>0.9935979677597592</v>
+        <v>0.9991873580268881</v>
       </c>
       <c r="AN101" t="n" s="83">
-        <v>0.0010504820834869135</v>
+        <v>0.9999678056601233</v>
       </c>
       <c r="AO101" t="n" s="83">
-        <v>0.9060992991137248</v>
+        <v>0.9730109320233835</v>
       </c>
       <c r="AP101" t="n" s="83">
-        <v>0.012119292155827192</v>
+        <v>0.9999999999996407</v>
       </c>
       <c r="AQ101" t="n" s="83">
         <v>1.7257851884373666E-23</v>
@@ -13651,25 +13651,25 @@
         <v>0.5</v>
       </c>
       <c r="AI102" t="n" s="83">
-        <v>0.9992184044676108</v>
+        <v>0.9990393470483632</v>
       </c>
       <c r="AJ102" t="n" s="83">
-        <v>0.9999992976079031</v>
+        <v>0.9999966381571442</v>
       </c>
       <c r="AK102" t="n" s="83">
-        <v>0.999999999999643</v>
+        <v>1.0</v>
       </c>
       <c r="AL102" t="n" s="83">
-        <v>0.9999459607947965</v>
+        <v>0.9997717002469008</v>
       </c>
       <c r="AM102" t="n" s="83">
-        <v>0.999999999999983</v>
+        <v>1.0</v>
       </c>
       <c r="AN102" t="n" s="83">
         <v>1.0</v>
       </c>
       <c r="AO102" t="n" s="83">
-        <v>0.9999245402669993</v>
+        <v>1.0</v>
       </c>
       <c r="AP102" t="n" s="83">
         <v>1.0</v>
@@ -13773,28 +13773,28 @@
         <v>0.5</v>
       </c>
       <c r="AI103" t="n" s="83">
-        <v>0.9924786881518278</v>
+        <v>0.9928630156556508</v>
       </c>
       <c r="AJ103" t="n" s="83">
-        <v>0.7317380900187286</v>
+        <v>0.8032405221195048</v>
       </c>
       <c r="AK103" t="n" s="83">
-        <v>0.003132520601195771</v>
+        <v>0.005948126918868547</v>
       </c>
       <c r="AL103" t="n" s="83">
-        <v>0.6320251269303754</v>
+        <v>0.6834337381051974</v>
       </c>
       <c r="AM103" t="n" s="83">
-        <v>0.022670037462673567</v>
+        <v>0.08225908961969843</v>
       </c>
       <c r="AN103" t="n" s="83">
-        <v>2.865556147062459E-16</v>
+        <v>5.059318781756419E-9</v>
       </c>
       <c r="AO103" t="n" s="83">
-        <v>0.18616334583406166</v>
+        <v>0.21346593381852227</v>
       </c>
       <c r="AP103" t="n" s="83">
-        <v>1.1774710088211215E-12</v>
+        <v>3.1119517383180765E-12</v>
       </c>
       <c r="AQ103" t="n" s="83">
         <v>2.9530768064434952E-46</v>
@@ -13895,28 +13895,28 @@
         <v>0.5</v>
       </c>
       <c r="AI104" t="n" s="83">
-        <v>0.999074525592067</v>
+        <v>0.9991221140378636</v>
       </c>
       <c r="AJ104" t="n" s="83">
-        <v>0.9867845180016819</v>
+        <v>0.9914444741397884</v>
       </c>
       <c r="AK104" t="n" s="83">
-        <v>0.7952839058475079</v>
+        <v>0.9544490875773297</v>
       </c>
       <c r="AL104" t="n" s="83">
-        <v>0.9929869822369769</v>
+        <v>0.9949693701453327</v>
       </c>
       <c r="AM104" t="n" s="83">
-        <v>0.9832691277016412</v>
+        <v>0.9975141346003857</v>
       </c>
       <c r="AN104" t="n" s="83">
-        <v>0.034737052874623434</v>
+        <v>1.0</v>
       </c>
       <c r="AO104" t="n" s="83">
-        <v>0.7592612854208179</v>
+        <v>0.8025091839003786</v>
       </c>
       <c r="AP104" t="n" s="83">
-        <v>3.9054555442615154E-4</v>
+        <v>0.0015574009813698702</v>
       </c>
       <c r="AQ104" t="n" s="83">
         <v>2.6476673564123678E-22</v>
@@ -14017,28 +14017,28 @@
         <v>0.5</v>
       </c>
       <c r="AI105" t="n" s="83">
-        <v>0.9989933996778886</v>
+        <v>0.9990451556796934</v>
       </c>
       <c r="AJ105" t="n" s="83">
-        <v>0.9424627242890665</v>
+        <v>0.9621517068582951</v>
       </c>
       <c r="AK105" t="n" s="83">
-        <v>0.0754181349899714</v>
+        <v>0.13783232897149583</v>
       </c>
       <c r="AL105" t="n" s="83">
-        <v>0.9765372268261889</v>
+        <v>0.9825155830315134</v>
       </c>
       <c r="AM105" t="n" s="83">
-        <v>0.8980771127548363</v>
+        <v>0.9805179990278212</v>
       </c>
       <c r="AN105" t="n" s="83">
-        <v>5.854038711249399E-10</v>
+        <v>0.013563279085763193</v>
       </c>
       <c r="AO105" t="n" s="83">
-        <v>0.7300873886108452</v>
+        <v>0.772482979257929</v>
       </c>
       <c r="AP105" t="n" s="83">
-        <v>1.7509015977300392E-7</v>
+        <v>6.156032875184385E-7</v>
       </c>
       <c r="AQ105" t="n" s="83">
         <v>1.4658832734971673E-37</v>

</xml_diff>